<commit_message>
Auto commit - 02021731
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$12</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-02  )</t>
   </si>
@@ -441,6 +441,45 @@
   </si>
   <si>
     <t>PMQ1+7210002837</t>
+  </si>
+  <si>
+    <t>14770115020201</t>
+  </si>
+  <si>
+    <t>中和嘉德店</t>
+  </si>
+  <si>
+    <t>2026-02-02 16:44:55</t>
+  </si>
+  <si>
+    <t>HL34</t>
+  </si>
+  <si>
+    <t>HL-HUB</t>
+  </si>
+  <si>
+    <t>HUB週期維護</t>
+  </si>
+  <si>
+    <t>2026年1月份 hub調查異常：PING91不通無法連線HUB，其他線路正常</t>
+  </si>
+  <si>
+    <t>THILF04770</t>
+  </si>
+  <si>
+    <t>2026-02-02 16:45:19</t>
+  </si>
+  <si>
+    <t>2026-02-02 16:12:00</t>
+  </si>
+  <si>
+    <t>2026-02-02 16:48:00</t>
+  </si>
+  <si>
+    <t>2026-02-03 20:45:00</t>
+  </si>
+  <si>
+    <t>Hub重置設定 已請0800檢查連線正常+HUB</t>
   </si>
 </sst>
 </file>
@@ -854,10 +893,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK11"/>
+  <dimension ref="A1:AK12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1799,7 +1838,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="7"/>
       <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
+      <c r="P11" s="9"/>
       <c r="Q11" s="7" t="s">
         <v>109</v>
       </c>
@@ -1832,7 +1871,7 @@
       <c r="AB11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC11" s="8" t="s">
+      <c r="AC11" s="9" t="s">
         <v>136</v>
       </c>
       <c r="AD11" s="7" t="s">
@@ -1845,6 +1884,103 @@
       <c r="AI11" s="7"/>
       <c r="AJ11" s="7"/>
       <c r="AK11" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2026020372</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4770</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N12" s="3">
+        <v>3404</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T12" s="3">
+        <v>1</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC12" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02031821
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$16</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="150">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-02  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="185">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-03  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -480,6 +480,113 @@
   </si>
   <si>
     <t>Hub重置設定 已請0800檢查連線正常+HUB</t>
+  </si>
+  <si>
+    <t>15197115020301</t>
+  </si>
+  <si>
+    <t>蘆洲鴻悅店</t>
+  </si>
+  <si>
+    <t>新北市蘆洲區</t>
+  </si>
+  <si>
+    <t>2026-02-03 09:09:09</t>
+  </si>
+  <si>
+    <t>星期二</t>
+  </si>
+  <si>
+    <t>HL60</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET印票機L90</t>
+  </si>
+  <si>
+    <t>切刀卡紙，切紙不正常</t>
+  </si>
+  <si>
+    <t>門市反應MMK印票機L90列印出的票券位置不正確，另表示TM刷讀小白單後需等待1分鐘以上才會出票卷，已有關機紙捲重裝仍異常。01/06台芝到店調整定位齒輪 重裝韌體...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05197</t>
+  </si>
+  <si>
+    <t>2026-02-03 09:13:45</t>
+  </si>
+  <si>
+    <t>2026-02-03 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-03 14:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:13:00</t>
+  </si>
+  <si>
+    <t>更換印票機
+換上8139003082
+換下8139003120</t>
+  </si>
+  <si>
+    <t>中和力德店</t>
+  </si>
+  <si>
+    <t>THILF04008</t>
+  </si>
+  <si>
+    <t>2026-02-03 11:21:22</t>
+  </si>
+  <si>
+    <t>2026-02-03 10:55:00</t>
+  </si>
+  <si>
+    <t>2026-02-03 11:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002970</t>
+  </si>
+  <si>
+    <t>蘆竹南福店</t>
+  </si>
+  <si>
+    <t>桃園市蘆竹區</t>
+  </si>
+  <si>
+    <t>THILF04272</t>
+  </si>
+  <si>
+    <t>2026-02-03 15:04:44</t>
+  </si>
+  <si>
+    <t>2026-02-03 14:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-03 15:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002736+L90</t>
+  </si>
+  <si>
+    <t>龜山崇優店</t>
+  </si>
+  <si>
+    <t>桃園市龜山區</t>
+  </si>
+  <si>
+    <t>THILF04197</t>
+  </si>
+  <si>
+    <t>2026-02-03 15:54:35</t>
+  </si>
+  <si>
+    <t>2026-02-03 15:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-03 15:53:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002706+L90</t>
   </si>
 </sst>
 </file>
@@ -893,10 +1000,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK12"/>
+  <dimension ref="A1:AK16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC9" sqref="AC9"/>
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1933,7 +2040,7 @@
       <c r="O12" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="10" t="s">
         <v>143</v>
       </c>
       <c r="Q12" s="3" t="s">
@@ -1970,7 +2077,7 @@
       <c r="AB12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC12" s="4" t="s">
+      <c r="AC12" s="10" t="s">
         <v>149</v>
       </c>
       <c r="AD12" s="3"/>
@@ -1981,6 +2088,336 @@
       <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="A13" s="7">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2026020414</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="7">
+        <v>5197</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="N13" s="7">
+        <v>6001</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="R13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T13" s="7">
+        <v>1</v>
+      </c>
+      <c r="U13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V13" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="W13" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y13" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC13" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2026020448</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>4008</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T14" s="3">
+        <v>1</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC14" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2026020528</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7">
+        <v>4272</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T15" s="7">
+        <v>1</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2026020582</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>4197</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC16" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02041140
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$17</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="185">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-03  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="200">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-04  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -587,6 +587,51 @@
   </si>
   <si>
     <t>PMQ1+7210002706+L90</t>
+  </si>
+  <si>
+    <t>E3052115020401</t>
+  </si>
+  <si>
+    <t>新莊莊玲店</t>
+  </si>
+  <si>
+    <t>2026-02-04 09:48:39</t>
+  </si>
+  <si>
+    <t>星期三</t>
+  </si>
+  <si>
+    <t>HLF3</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET QRcode掃描器</t>
+  </si>
+  <si>
+    <t>F301</t>
+  </si>
+  <si>
+    <t>掃描無反應或感應不良</t>
+  </si>
+  <si>
+    <t>門市反應MMK 四代機 QRCODE掃描器刷讀QRCODE有亮紅光但無反應(例:餐食券...)，已有重新開機仍異常(掃描後無反應也沒出紙)</t>
+  </si>
+  <si>
+    <t>THILF03052</t>
+  </si>
+  <si>
+    <t>2026-02-04 09:58:52</t>
+  </si>
+  <si>
+    <t>2026-02-04 10:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:58:00</t>
+  </si>
+  <si>
+    <t>現場測試正常</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1045,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK16"/>
+  <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC13" sqref="AC13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2372,7 +2417,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="3"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="P16" s="10"/>
       <c r="Q16" s="3" t="s">
         <v>180</v>
       </c>
@@ -2405,7 +2450,7 @@
       <c r="AB16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC16" s="4" t="s">
+      <c r="AC16" s="10" t="s">
         <v>184</v>
       </c>
       <c r="AD16" s="3" t="s">
@@ -2418,6 +2463,103 @@
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2026020765</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="7">
+        <v>3052</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T17" s="7">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z17" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC17" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="7"/>
+      <c r="AK17" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02051839
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$41</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="200">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-04  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="363">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-05  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -632,6 +632,508 @@
   </si>
   <si>
     <t>現場測試正常</t>
+  </si>
+  <si>
+    <t>E2042115020401</t>
+  </si>
+  <si>
+    <t>三重中央北店</t>
+  </si>
+  <si>
+    <t>2026-02-04 09:47:00</t>
+  </si>
+  <si>
+    <t>HL25</t>
+  </si>
+  <si>
+    <t>HL-SC螢幕</t>
+  </si>
+  <si>
+    <t>螢幕畫面閃爍頻繁或無畫面</t>
+  </si>
+  <si>
+    <t>門市反應sc螢幕(LCD22)畫面有波浪紋跳動，門市已有重新拔插後方線路仍異常....須請台芝到店協助(畫面會抖動)
+02/04 09:58 門市告知目前盤點沒空，會再進電協助....李</t>
+  </si>
+  <si>
+    <t>THILF02042</t>
+  </si>
+  <si>
+    <t>2026-02-04 12:15:20</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 16:15:00</t>
+  </si>
+  <si>
+    <t>VGA線對接螢幕sc主機沒破浪紋.
+VG A線接切換器就會有波浪紋</t>
+  </si>
+  <si>
+    <t>龜山復興店</t>
+  </si>
+  <si>
+    <t>THILF05075</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:19:34</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:18:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002716+L90</t>
+  </si>
+  <si>
+    <t>龜山慧敏店</t>
+  </si>
+  <si>
+    <t>THILF05248</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:54:59</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:49:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002718</t>
+  </si>
+  <si>
+    <t>L533</t>
+  </si>
+  <si>
+    <t>田倉復興店</t>
+  </si>
+  <si>
+    <t>THILF0L533</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:14:26</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:14:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:37:26</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 13:55:00</t>
+  </si>
+  <si>
+    <t>+L90無法移動</t>
+  </si>
+  <si>
+    <t>龜山文化七</t>
+  </si>
+  <si>
+    <t>THILF05031</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:42:09</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:20:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:41:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002715+L90</t>
+  </si>
+  <si>
+    <t>1D609115020401</t>
+  </si>
+  <si>
+    <t>D609</t>
+  </si>
+  <si>
+    <t>板橋大興店</t>
+  </si>
+  <si>
+    <t>新北市板橋區</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:09:15</t>
+  </si>
+  <si>
+    <t>HLF2</t>
+  </si>
+  <si>
+    <t>HL-CCD掃描器(TM)</t>
+  </si>
+  <si>
+    <t>F201</t>
+  </si>
+  <si>
+    <t>門市反應TM1掃描槍(HC76 TR)刷讀行動條碼與商品都無反應，確認有亮燈有逼聲、鼠標有在輸入的位置，執行掃槍校正時刷讀到第6條碼就沒反應...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D609</t>
+  </si>
+  <si>
+    <t>狄澤洋</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:11:48</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:20:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 19:11:00</t>
+  </si>
+  <si>
+    <t>更換76掃槍
+換上：8119013216
+換下：8119010876</t>
+  </si>
+  <si>
+    <t>eS-3008A 黑白複合機</t>
+  </si>
+  <si>
+    <t>龜山香品店</t>
+  </si>
+  <si>
+    <t>THILF03008</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:20:15</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:19:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002701+L90</t>
+  </si>
+  <si>
+    <t>L534</t>
+  </si>
+  <si>
+    <t>田倉文興店</t>
+  </si>
+  <si>
+    <t>THILF0L534</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:34:43</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:37:34</t>
+  </si>
+  <si>
+    <t>2026-02-04 14:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002758</t>
+  </si>
+  <si>
+    <t>12540115020401</t>
+  </si>
+  <si>
+    <t>蘆竹坑子口</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:40:16</t>
+  </si>
+  <si>
+    <t>門市反應TM1 CCD掃描器(HC56II TR、HC76 TR)接頭處脫牙，線路鬆脫導致掃槍感應不良無法刷讀...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02540</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:43:49</t>
+  </si>
+  <si>
+    <t>2026-02-05 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 19:43:00</t>
+  </si>
+  <si>
+    <t>鎖上螺絲後確認無脫落可正常使用</t>
+  </si>
+  <si>
+    <t>12540115020402</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:44:08</t>
+  </si>
+  <si>
+    <t>門市反應TM2掃描槍(HC56II TR、HC76 TR)刷讀發財卡與代收條碼經常無反應，確認有亮燈有逼聲、鼠標有在輸入的位置，2/3已執行掃槍校正仍異常...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-02-04 15:46:53</t>
+  </si>
+  <si>
+    <t>2026-02-05 19:46:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119006210
+換上8119011149
+更換IO版</t>
+  </si>
+  <si>
+    <t>龜山A8站</t>
+  </si>
+  <si>
+    <t>THILF05402</t>
+  </si>
+  <si>
+    <t>2026-02-04 16:45:24</t>
+  </si>
+  <si>
+    <t>2026-02-04 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-04 16:44:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002719+L90無法移動</t>
+  </si>
+  <si>
+    <t>14552115020401</t>
+  </si>
+  <si>
+    <t>新莊福慧店</t>
+  </si>
+  <si>
+    <t>2026-02-04 17:09:56</t>
+  </si>
+  <si>
+    <t>2026/01HUB週期維護:PING全店通，連線至hub白畫面</t>
+  </si>
+  <si>
+    <t>THILF04552</t>
+  </si>
+  <si>
+    <t>2026-02-04 17:10:59</t>
+  </si>
+  <si>
+    <t>2026-02-04 17:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 21:11:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+HUB
+更換HUB
+換上8107005250
+換下8107004021
+</t>
+  </si>
+  <si>
+    <t>2026-02-04 17:16:16</t>
+  </si>
+  <si>
+    <t>2026-02-04 17:15:00</t>
+  </si>
+  <si>
+    <t>中和和圓店</t>
+  </si>
+  <si>
+    <t>THILF02570</t>
+  </si>
+  <si>
+    <t>2026-02-05 11:41:17</t>
+  </si>
+  <si>
+    <t>2026-02-05 10:47:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 11:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002964</t>
+  </si>
+  <si>
+    <t>14804115020502</t>
+  </si>
+  <si>
+    <t>三重國隆店</t>
+  </si>
+  <si>
+    <t>2026-02-05 12:00:07</t>
+  </si>
+  <si>
+    <t>星期四</t>
+  </si>
+  <si>
+    <t>觸控不良(游標偏移)</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控不良,確認無異物或是螢幕保護貼及廣告文宣影響,已有觸控校正仍無法排除,還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04804</t>
+  </si>
+  <si>
+    <t>2026-02-05 12:01:35</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:15:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:42:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 16:01:00</t>
+  </si>
+  <si>
+    <t>校正.重接排線.整理排線</t>
+  </si>
+  <si>
+    <t>中和泰和店</t>
+  </si>
+  <si>
+    <t>THILF02398</t>
+  </si>
+  <si>
+    <t>2026-02-05 12:14:29</t>
+  </si>
+  <si>
+    <t>2026-02-05 11:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 11:45:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002963</t>
+  </si>
+  <si>
+    <t>三重大仁店</t>
+  </si>
+  <si>
+    <t>THILF02543</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:23:43</t>
+  </si>
+  <si>
+    <t>2026-02-05 12:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:05:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002768</t>
+  </si>
+  <si>
+    <t>三重今大店</t>
+  </si>
+  <si>
+    <t>THILF04184</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:44:32</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:15:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002792</t>
+  </si>
+  <si>
+    <t>新莊瓊林南</t>
+  </si>
+  <si>
+    <t>THILF02109</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:54:32</t>
+  </si>
+  <si>
+    <t>2026-02-05 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:00:00</t>
+  </si>
+  <si>
+    <t>2109新莊瓊林南裝潢回裝已完工已回報0800
+現場使用中華電信
+商顯已安裝完工</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:42:02</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002807</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:47:07</t>
+  </si>
+  <si>
+    <t>2026-02-05 13:51:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:06:00</t>
+  </si>
+  <si>
+    <t>15428115020501</t>
+  </si>
+  <si>
+    <t>三重野球魂</t>
+  </si>
+  <si>
+    <t>2026-02-05 15:15:12</t>
+  </si>
+  <si>
+    <t>2026年1月份 hub調查異常：8PORT插在9PORT</t>
+  </si>
+  <si>
+    <t>THILF05428</t>
+  </si>
+  <si>
+    <t>2026-02-05 15:17:49</t>
+  </si>
+  <si>
+    <t>2026-02-05 14:55:00</t>
+  </si>
+  <si>
+    <t>2026-02-05 15:20:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 19:17:00</t>
+  </si>
+  <si>
+    <t>9port插回8port  已請0800連線檢查確認 +HUB</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1547,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK17"/>
+  <dimension ref="A1:AK41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2512,7 +3014,7 @@
       <c r="O17" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="P17" s="8" t="s">
+      <c r="P17" s="9" t="s">
         <v>193</v>
       </c>
       <c r="Q17" s="7" t="s">
@@ -2549,7 +3051,7 @@
       <c r="AB17" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC17" s="8" t="s">
+      <c r="AC17" s="9" t="s">
         <v>199</v>
       </c>
       <c r="AD17" s="7"/>
@@ -2560,6 +3062,2008 @@
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
       <c r="AK17" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2026020805</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2042</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="N18" s="3">
+        <v>2501</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC18" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2026020809</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7">
+        <v>5075</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T19" s="7">
+        <v>1</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC19" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2026020817</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>5248</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC20" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2026020823</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T21" s="7">
+        <v>1</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2026020827</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <v>5248</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC22" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK22" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2026020830</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7">
+        <v>5031</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7"/>
+      <c r="AK23" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2026020843</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y24" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC24" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2026020848</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="7">
+        <v>3008</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="AD25" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="7"/>
+      <c r="AK25" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2026020864</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T26" s="3">
+        <v>1</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC26" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2026020865</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7">
+        <v>2042</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE27" s="7"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK27" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2026020867</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2540</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="P28" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T28" s="3">
+        <v>1</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y28" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>5</v>
+      </c>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC28" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2026020869</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="7">
+        <v>2540</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T29" s="7">
+        <v>1</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y29" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="Z29" s="7">
+        <v>5</v>
+      </c>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC29" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD29" s="7"/>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="7"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="7"/>
+      <c r="AJ29" s="7"/>
+      <c r="AK29" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2026020876</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3">
+        <v>5402</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC30" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="AD30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="7">
+        <v>2026020898</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="7">
+        <v>4552</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N31" s="7">
+        <v>3404</v>
+      </c>
+      <c r="O31" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T31" s="7">
+        <v>1</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="W31" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="X31" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y31" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="Z31" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7"/>
+      <c r="AK31" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2026020900</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>4552</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T32" s="3">
+        <v>1</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC32" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK32" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2026021003</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7">
+        <v>2570</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="AD33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK33" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2026021020</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="3">
+        <v>4804</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N34" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="P34" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T34" s="3">
+        <v>1</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y34" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="Z34" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC34" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2026021025</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7">
+        <v>2398</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="R35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T35" s="7">
+        <v>1</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC35" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK35" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2026021032</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>2543</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T36" s="3">
+        <v>1</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="X36" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC36" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK36" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2026021038</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7">
+        <v>4184</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T37" s="7">
+        <v>1</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="X37" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC37" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="AD37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK37" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2026021040</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <v>2109</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T38" s="3">
+        <v>1</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC38" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF38" s="3"/>
+      <c r="AG38" s="3"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="3"/>
+      <c r="AK38" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2026021056</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7">
+        <v>4804</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T39" s="7">
+        <v>1</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V39" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="X39" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC39" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="AD39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK39" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2026021060</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T40" s="3">
+        <v>1</v>
+      </c>
+      <c r="U40" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC40" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD40" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="3"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3"/>
+    </row>
+    <row r="41" spans="1:37">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2026021074</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="7">
+        <v>5428</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N41" s="7">
+        <v>3404</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="R41" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T41" s="7">
+        <v>1</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V41" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="W41" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="X41" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="Z41" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA41" s="7"/>
+      <c r="AB41" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC41" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="AD41" s="7"/>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="7"/>
+      <c r="AK41" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02061740
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$52</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="363">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-05  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="436">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-06  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1134,6 +1134,232 @@
   </si>
   <si>
     <t>9port插回8port  已請0800連線檢查確認 +HUB</t>
+  </si>
+  <si>
+    <t>15457115020601</t>
+  </si>
+  <si>
+    <t>三重鑫五華</t>
+  </si>
+  <si>
+    <t>2026-02-06 10:09:16</t>
+  </si>
+  <si>
+    <t>HL24</t>
+  </si>
+  <si>
+    <t>HL-SC主機</t>
+  </si>
+  <si>
+    <t>檔案損毀(更換硬碟)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(SHUTTLE6S)2026/2/6 (週五) 上午 09:59 總公司明翰來信:有關5457三重鑫五華門市確認SC障礙問題。請協助一般派工，到店更換SC主機+第一、二顆硬碟，資料不備份，謝謝。PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認帳關到02/05，與通訊嘉芳確認02/05銷售都有收到
+</t>
+  </si>
+  <si>
+    <t>THILF05457</t>
+  </si>
+  <si>
+    <t>2026-02-06 10:24:41</t>
+  </si>
+  <si>
+    <t>2026-02-06 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 17:12:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 14:24:00</t>
+  </si>
+  <si>
+    <t>更換sc主機及第一 二 顆硬碟不備份還原
+換下8114004043換上8114004393
+SC = 20250805
+SC_Slave = 20250805
+HiPOS  最新版本=S113.62.0   ARC.DEF = ARC5.202u
+已跟店家宣達請門市先回報代收會計</t>
+  </si>
+  <si>
+    <t>北縣淡俊店</t>
+  </si>
+  <si>
+    <t>THILF02318</t>
+  </si>
+  <si>
+    <t>2026-02-06 12:28:53</t>
+  </si>
+  <si>
+    <t>2026-02-06 09:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 10:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002886</t>
+  </si>
+  <si>
+    <t>中和自治店</t>
+  </si>
+  <si>
+    <t>THILF03318</t>
+  </si>
+  <si>
+    <t>2026-02-06 12:29:37</t>
+  </si>
+  <si>
+    <t>2026-02-06 11:45:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 12:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002966</t>
+  </si>
+  <si>
+    <t>淡水台電宿舍</t>
+  </si>
+  <si>
+    <t>THILF02897</t>
+  </si>
+  <si>
+    <t>2026-02-06 12:30:04</t>
+  </si>
+  <si>
+    <t>2026-02-06 10:20:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 10:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002888</t>
+  </si>
+  <si>
+    <t>A171</t>
+  </si>
+  <si>
+    <t>淡水金龍店</t>
+  </si>
+  <si>
+    <t>THILF0A171</t>
+  </si>
+  <si>
+    <t>2026-02-06 12:30:39</t>
+  </si>
+  <si>
+    <t>2026-02-06 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 11:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003049</t>
+  </si>
+  <si>
+    <t>淡水後洲店</t>
+  </si>
+  <si>
+    <t>THILF04298</t>
+  </si>
+  <si>
+    <t>2026-02-06 13:34:16</t>
+  </si>
+  <si>
+    <t>2026-02-06 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 13:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002892</t>
+  </si>
+  <si>
+    <t>淡水新洲店</t>
+  </si>
+  <si>
+    <t>THILF04529</t>
+  </si>
+  <si>
+    <t>2026-02-06 13:58:14</t>
+  </si>
+  <si>
+    <t>2026-02-06 13:35:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 13:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002894</t>
+  </si>
+  <si>
+    <t>淡水海天店</t>
+  </si>
+  <si>
+    <t>THILF04541</t>
+  </si>
+  <si>
+    <t>2026-02-06 14:27:32</t>
+  </si>
+  <si>
+    <t>2026-02-06 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 14:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002895</t>
+  </si>
+  <si>
+    <t>淡水新市一</t>
+  </si>
+  <si>
+    <t>THILF04093</t>
+  </si>
+  <si>
+    <t>2026-02-06 15:24:41</t>
+  </si>
+  <si>
+    <t>2026-02-06 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 15:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002890</t>
+  </si>
+  <si>
+    <t>淡水沙崙店</t>
+  </si>
+  <si>
+    <t>THILF04802</t>
+  </si>
+  <si>
+    <t>2026-02-06 15:50:50</t>
+  </si>
+  <si>
+    <t>2026-02-06 15:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003046</t>
+  </si>
+  <si>
+    <t>淡水魚市店</t>
+  </si>
+  <si>
+    <t>THILF05060</t>
+  </si>
+  <si>
+    <t>2026-02-06 16:22:05</t>
+  </si>
+  <si>
+    <t>2026-02-06 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-06 16:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003047</t>
   </si>
 </sst>
 </file>
@@ -1547,10 +1773,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK41"/>
+  <dimension ref="A1:AK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="AC49" sqref="AC49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5016,7 +5242,7 @@
       <c r="O41" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="P41" s="8" t="s">
+      <c r="P41" s="9" t="s">
         <v>356</v>
       </c>
       <c r="Q41" s="7" t="s">
@@ -5053,7 +5279,7 @@
       <c r="AB41" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC41" s="8" t="s">
+      <c r="AC41" s="9" t="s">
         <v>362</v>
       </c>
       <c r="AD41" s="7"/>
@@ -5064,6 +5290,875 @@
       <c r="AI41" s="7"/>
       <c r="AJ41" s="7"/>
       <c r="AK41" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2026021139</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="3">
+        <v>5457</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="N42" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T42" s="3">
+        <v>1</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC42" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="3"/>
+      <c r="AG42" s="3"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="3"/>
+      <c r="AJ42" s="3"/>
+      <c r="AK42" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2026021213</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7">
+        <v>2318</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="R43" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T43" s="7">
+        <v>1</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V43" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="W43" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="X43" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="Y43" s="7"/>
+      <c r="Z43" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC43" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="AD43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE43" s="7"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2026021214</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
+        <v>3318</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T44" s="3">
+        <v>1</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC44" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="AD44" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
+      <c r="AG44" s="3"/>
+      <c r="AH44" s="3"/>
+      <c r="AI44" s="3"/>
+      <c r="AJ44" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK44" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2026021215</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7">
+        <v>2897</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="R45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S45" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T45" s="7">
+        <v>1</v>
+      </c>
+      <c r="U45" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V45" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="W45" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="X45" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC45" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="AD45" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE45" s="7"/>
+      <c r="AF45" s="7"/>
+      <c r="AG45" s="7"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7"/>
+      <c r="AJ45" s="7"/>
+      <c r="AK45" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2026021216</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T46" s="3">
+        <v>1</v>
+      </c>
+      <c r="U46" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC46" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="3"/>
+      <c r="AG46" s="3"/>
+      <c r="AH46" s="3"/>
+      <c r="AI46" s="3"/>
+      <c r="AJ46" s="3"/>
+      <c r="AK46" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="7">
+        <v>2026021219</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7">
+        <v>4298</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T47" s="7">
+        <v>1</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="W47" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="X47" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC47" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="AD47" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
+      <c r="AG47" s="7"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="7"/>
+      <c r="AJ47" s="7"/>
+      <c r="AK47" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="3">
+        <v>2026021236</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3">
+        <v>4529</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T48" s="3">
+        <v>1</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC48" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="3"/>
+      <c r="AK48" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="7">
+        <v>2026021246</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7">
+        <v>4541</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="R49" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T49" s="7">
+        <v>1</v>
+      </c>
+      <c r="U49" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="W49" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="X49" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC49" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="AD49" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE49" s="7"/>
+      <c r="AF49" s="7"/>
+      <c r="AG49" s="7"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="7"/>
+      <c r="AJ49" s="7"/>
+      <c r="AK49" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2026021351</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3">
+        <v>4093</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T50" s="3">
+        <v>1</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V50" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="X50" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC50" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="AD50" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE50" s="3"/>
+      <c r="AF50" s="3"/>
+      <c r="AG50" s="3"/>
+      <c r="AH50" s="3"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="3"/>
+      <c r="AK50" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="7">
+        <v>2026021364</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7">
+        <v>4802</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T51" s="7">
+        <v>1</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="W51" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC51" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="AD51" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="7"/>
+      <c r="AK51" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2026021376</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>5060</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T52" s="3">
+        <v>1</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC52" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="AD52" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE52" s="3"/>
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="3"/>
+      <c r="AH52" s="3"/>
+      <c r="AI52" s="3"/>
+      <c r="AJ52" s="3"/>
+      <c r="AK52" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02101729
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$77</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="436">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-06  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="625">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-10  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1360,6 +1360,593 @@
   </si>
   <si>
     <t>PMQ1+7210003047</t>
+  </si>
+  <si>
+    <t>E4163115020601</t>
+  </si>
+  <si>
+    <t>新莊中泉店</t>
+  </si>
+  <si>
+    <t>2026-02-06 18:29:46</t>
+  </si>
+  <si>
+    <t>D302</t>
+  </si>
+  <si>
+    <t>發票印字不清</t>
+  </si>
+  <si>
+    <t>門市反應TM1熱感發票機(BSC10II)列印皆出現直條白線並會遮擋序號，已有重關機更換新紙捲仍異常...需請台芝到店(印字不清 中間空格)</t>
+  </si>
+  <si>
+    <t>THILF04163</t>
+  </si>
+  <si>
+    <t>2026-02-06 18:41:50</t>
+  </si>
+  <si>
+    <t>2026-02-09 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 10:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 22:41:00</t>
+  </si>
+  <si>
+    <t>清潔印字頭</t>
+  </si>
+  <si>
+    <t>E3853115020701</t>
+  </si>
+  <si>
+    <t>板橋互助店</t>
+  </si>
+  <si>
+    <t>2026-02-07 08:12:28</t>
+  </si>
+  <si>
+    <t>星期六</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控不良，都要點選很多次才有反應，門市告知超級繁忙無法協助觸控校正，與門市確認螢幕無貼保護貼、文宣....請台芝到店協助(sos)</t>
+  </si>
+  <si>
+    <t>THILF03853</t>
+  </si>
+  <si>
+    <t>2026-02-07 09:13:36</t>
+  </si>
+  <si>
+    <t>2026-02-10 10:45:00</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:19:00</t>
+  </si>
+  <si>
+    <t>2026-02-10 13:00:00</t>
+  </si>
+  <si>
+    <t>線路重新整理、驅動程式校正後測試正常</t>
+  </si>
+  <si>
+    <t>13853115020701</t>
+  </si>
+  <si>
+    <t>2026-02-07 09:04:02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM1 CCD掃描器(HC76TR)刷讀所有條碼都感應不良，要刷很多次才有反應，已有執行校正仍異常....請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>2026-02-07 09:14:04</t>
+  </si>
+  <si>
+    <t>掃槍校正後測試正常</t>
+  </si>
+  <si>
+    <t>13853115020702</t>
+  </si>
+  <si>
+    <t>2026-02-07 09:04:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM2 CCD掃描器(HC76TR)刷讀所有條碼都感應不良，要刷很多次才有反應，已有執行校正仍異常....請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>2026-02-07 09:14:26</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:18:00</t>
+  </si>
+  <si>
+    <t>14528115020701</t>
+  </si>
+  <si>
+    <t>急修件</t>
+  </si>
+  <si>
+    <t>八里鐵塔店</t>
+  </si>
+  <si>
+    <t>新北市八里區</t>
+  </si>
+  <si>
+    <t>2026-02-07 11:18:10</t>
+  </si>
+  <si>
+    <t>當機</t>
+  </si>
+  <si>
+    <t>02/07 11:25 與總公司明翰確認啟動緊急叫修:門市告知TM1(TCX800)這兩天清帳或交班後黑屏無法開機，右下角燈號為紅燈，按了電源鍵都無反應，門市今日已更換到白色插座進行清帳後仍異常，已造成門市困擾...請台芝到店協助已與門市確認2/8無銷售PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計2.請確認SC的代收資料是否正確(須與代收單據逐一核對)</t>
+  </si>
+  <si>
+    <t>THILF04528</t>
+  </si>
+  <si>
+    <t>2026-02-07 11:32:15</t>
+  </si>
+  <si>
+    <t>2026-02-07 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-07 16:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-07 17:32:00</t>
+  </si>
+  <si>
+    <t>關機狀態按開機鍵無法開機，門市交班無法重啟
+更換主機，無更換硬碟沿用
+換下8185002181
+換上8185000524</t>
+  </si>
+  <si>
+    <t>1D191115020701</t>
+  </si>
+  <si>
+    <t>D191</t>
+  </si>
+  <si>
+    <t>三重興德店</t>
+  </si>
+  <si>
+    <t>2026-02-07 12:37:52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應tm2(TCX800)清帳後黑屏，帳條有出，電源燈亮藍燈按壓無法關機，請門市將線路重插後畫面顯示自動修復又跳回黑屏，電源燈仍藍燈，ping81不通無法vnc....請台芝到店協助
+已與門市確認02/07清帳後就無法開機，無交易PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)																																
+</t>
+  </si>
+  <si>
+    <t>THILF0D191</t>
+  </si>
+  <si>
+    <t>2026-02-07 12:41:02</t>
+  </si>
+  <si>
+    <t>2026-02-09 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 15:30:00</t>
+  </si>
+  <si>
+    <t>更換tm2第一顆硬碟不備份還原
+已請客服確認T M版本
+並告知店長回報代收</t>
+  </si>
+  <si>
+    <t>E4008115020701</t>
+  </si>
+  <si>
+    <t>2026-02-07 13:13:52</t>
+  </si>
+  <si>
+    <t>門市反應SC螢幕(LCD20)有一道明顯的裂痕以及右半邊有許多小線條，PING1通VNC畫面正常，請門市重新拔插後方線路仍異常..請台芝到店協助(電腦螢幕損壞，螢幕一半是黑的。)
+02/07 13:30   請門市拔插休息，稍晚聯繫...廖
+02/07 13:22.13:28 致電門市未接</t>
+  </si>
+  <si>
+    <t>2026-02-07 13:44:42</t>
+  </si>
+  <si>
+    <t>2026-02-09 17:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 17:30:00</t>
+  </si>
+  <si>
+    <t>換下8133003211. 換上8133003295</t>
+  </si>
+  <si>
+    <t>EF777115020701</t>
+  </si>
+  <si>
+    <t>F777</t>
+  </si>
+  <si>
+    <t>蘆竹南華店</t>
+  </si>
+  <si>
+    <t>2026-02-07 23:31:51</t>
+  </si>
+  <si>
+    <t>HL59</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET熱感機T70II</t>
+  </si>
+  <si>
+    <t>無反應，不會轉動</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應LIFEET熱感機T70II無反應，有亮紅燈，已有關機紙捲重裝仍異常...請台芝到店協助(卡紙無法列印)
+</t>
+  </si>
+  <si>
+    <t>THILF0F777</t>
+  </si>
+  <si>
+    <t>2026-02-08 09:10:46</t>
+  </si>
+  <si>
+    <t>2026-02-09 13:12:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 13:42:00</t>
+  </si>
+  <si>
+    <t>更換出單機
+換下8138002119
+換上8138002421</t>
+  </si>
+  <si>
+    <t>14155115020801</t>
+  </si>
+  <si>
+    <t>三重穀保店</t>
+  </si>
+  <si>
+    <t>2026-02-08 09:17:41</t>
+  </si>
+  <si>
+    <t>當機/自動開關機</t>
+  </si>
+  <si>
+    <t>02/08 09:18 啟動緊急叫修:門市反應稍早sc(SHUTTLE6S)畫面跳出磁碟修復的訊息無法開機，重啟多次關機休息後可正常開機但無法開啟訂貨3.0、hishop可開啟但無法操作其他功能畫面都會卡住，協助再次重啟卡再關機中無反應，請門市強制重啟後ping1通無法vnc，與門市確認訂貨3.0、hishop無法開啟.....須請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+與門市確認帳關到02/07，與通訊功評確認缺少tm1、2電子存根聯</t>
+  </si>
+  <si>
+    <t>THILF04155</t>
+  </si>
+  <si>
+    <t>2026-02-08 09:25:26</t>
+  </si>
+  <si>
+    <t>2026-02-08 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-08 14:32:00</t>
+  </si>
+  <si>
+    <t>2026-02-08 15:25:00</t>
+  </si>
+  <si>
+    <t>SC更換第一顆及第二顆硬碟進行不備份還原
+更換Sata線*2條</t>
+  </si>
+  <si>
+    <t>15074115020801</t>
+  </si>
+  <si>
+    <t>八里福德新村</t>
+  </si>
+  <si>
+    <t>2026-02-08 15:04:08</t>
+  </si>
+  <si>
+    <t>門市反應TM2 CCD掃描槍(HC56II TR、HC76 TR)無亮燈無逼聲無法刷讀，已嘗試重啟TM與發票機都只有閃一下燈就沒反應...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05074</t>
+  </si>
+  <si>
+    <t>2026-02-08 15:06:28</t>
+  </si>
+  <si>
+    <t>2026-02-09 10:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 11:20:00</t>
+  </si>
+  <si>
+    <t>#更正報修內容為TM1機台
+#現場測試信用卡機 多卡機及掃描槍都無反應，目前更換IO卡測試正常</t>
+  </si>
+  <si>
+    <t>2026-02-09 10:54:33</t>
+  </si>
+  <si>
+    <t>2026-02-09 10:45:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003061</t>
+  </si>
+  <si>
+    <t>新莊莊美店</t>
+  </si>
+  <si>
+    <t>THILF04341</t>
+  </si>
+  <si>
+    <t>2026-02-09 11:08:12</t>
+  </si>
+  <si>
+    <t>2026-02-09 10:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 11:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003064</t>
+  </si>
+  <si>
+    <t>北縣莊勝店</t>
+  </si>
+  <si>
+    <t>THILF03380</t>
+  </si>
+  <si>
+    <t>2026-02-09 11:24:11</t>
+  </si>
+  <si>
+    <t>2026-02-09 11:15:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 11:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003054</t>
+  </si>
+  <si>
+    <t>15513115020901</t>
+  </si>
+  <si>
+    <t>新莊A3站</t>
+  </si>
+  <si>
+    <t>2026-02-09 14:32:35</t>
+  </si>
+  <si>
+    <t>2026年01月份 HUB週期維護	PING91不通無法連線HUB，其他線路正常</t>
+  </si>
+  <si>
+    <t>THILF05513</t>
+  </si>
+  <si>
+    <t>2026-02-09 14:33:08</t>
+  </si>
+  <si>
+    <t>2026-02-09 14:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 14:45:00</t>
+  </si>
+  <si>
+    <t>2026-02-10 18:33:00</t>
+  </si>
+  <si>
+    <t>重設HUB 回報0800測試正常</t>
+  </si>
+  <si>
+    <t>龜山南上店</t>
+  </si>
+  <si>
+    <t>THILF04035</t>
+  </si>
+  <si>
+    <t>2026-02-09 14:33:45</t>
+  </si>
+  <si>
+    <t>2026-02-09 13:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-09 14:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002705+L90</t>
+  </si>
+  <si>
+    <t>蘆竹南山北</t>
+  </si>
+  <si>
+    <t>THILF05357</t>
+  </si>
+  <si>
+    <t>2026-02-09 15:41:28</t>
+  </si>
+  <si>
+    <t>2026-02-09 15:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002743+L90</t>
+  </si>
+  <si>
+    <t>E4601115021001</t>
+  </si>
+  <si>
+    <t>蘆竹領航店</t>
+  </si>
+  <si>
+    <t>2026-02-10 09:12:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM1掃描器(HC56II-TR)常常刷讀無反應有亮燈有逼聲，請門市操作掃描器校正第一段條碼刷完無亮燈後續條碼也都刷不出來....須請台芝到店協助(CCD掃描器常常刷讀不到條碼)
+02/10  09:22 請門市先執行掃描器校正，稍晚聯繫...廖
+</t>
+  </si>
+  <si>
+    <t>THILF04601</t>
+  </si>
+  <si>
+    <t>2026-02-10 09:43:54</t>
+  </si>
+  <si>
+    <t>2026-02-10 13:55:00</t>
+  </si>
+  <si>
+    <t>2026-02-10 14:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-11 13:43:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119010427
+換上8119006641</t>
+  </si>
+  <si>
+    <t>12380115021001</t>
+  </si>
+  <si>
+    <t>永和樂華夜市</t>
+  </si>
+  <si>
+    <t>新北市永和區</t>
+  </si>
+  <si>
+    <t>2026-02-10 10:08:38</t>
+  </si>
+  <si>
+    <t>F604</t>
+  </si>
+  <si>
+    <t>無電源反應</t>
+  </si>
+  <si>
+    <t>門市反應稍早跳電後TM1多卡機(QP3000E)無電源反應黑屏，後方線路雜亂無法重新拔插....須請台芝到店協住</t>
+  </si>
+  <si>
+    <t>THILF02380</t>
+  </si>
+  <si>
+    <t>2026-02-10 10:10:13</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:05:00</t>
+  </si>
+  <si>
+    <t>2026-02-11 14:10:00</t>
+  </si>
+  <si>
+    <t>整理排線.重新插拔</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:21:55</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:17:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002852</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:39:55</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:25:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002985</t>
+  </si>
+  <si>
+    <t>C192</t>
+  </si>
+  <si>
+    <t>北縣福美店</t>
+  </si>
+  <si>
+    <t>THILF0C192</t>
+  </si>
+  <si>
+    <t>2026-02-10 12:43:57</t>
+  </si>
+  <si>
+    <t>2026-02-10 11:55:00</t>
+  </si>
+  <si>
+    <t>2026-02-10 12:25:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002979+L90</t>
+  </si>
+  <si>
+    <t>2026-02-10 14:31:26</t>
+  </si>
+  <si>
+    <t>2026-02-10 14:30:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002740+L90</t>
+  </si>
+  <si>
+    <t>新莊豐年店</t>
+  </si>
+  <si>
+    <t>THILF02743</t>
+  </si>
+  <si>
+    <t>2026-02-10 15:24:05</t>
+  </si>
+  <si>
+    <t>2026-02-10 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-10 15:15:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003051</t>
+  </si>
+  <si>
+    <t>新莊瓊泰店</t>
+  </si>
+  <si>
+    <t>THILF04208</t>
+  </si>
+  <si>
+    <t>2026-02-10 15:52:15</t>
+  </si>
+  <si>
+    <t>2026-02-10 15:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-10 15:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003063</t>
+  </si>
+  <si>
+    <t>L551</t>
+  </si>
+  <si>
+    <t>林口顧家店</t>
+  </si>
+  <si>
+    <t>新北市林口區</t>
+  </si>
+  <si>
+    <t>THILF0L551</t>
+  </si>
+  <si>
+    <t>2026-02-10 15:56:53</t>
+  </si>
+  <si>
+    <t>2026-02-10 16:00:00</t>
+  </si>
+  <si>
+    <t>閉店撤機完成</t>
   </si>
 </sst>
 </file>
@@ -1773,10 +2360,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK52"/>
+  <dimension ref="A1:AK77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC49" sqref="AC49"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6113,7 +6700,7 @@
       <c r="M52" s="4"/>
       <c r="N52" s="3"/>
       <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
+      <c r="P52" s="10"/>
       <c r="Q52" s="3" t="s">
         <v>431</v>
       </c>
@@ -6146,7 +6733,7 @@
       <c r="AB52" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC52" s="4" t="s">
+      <c r="AC52" s="10" t="s">
         <v>435</v>
       </c>
       <c r="AD52" s="3" t="s">
@@ -6159,6 +6746,2201 @@
       <c r="AI52" s="3"/>
       <c r="AJ52" s="3"/>
       <c r="AK52" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="7">
+        <v>2026021427</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="7">
+        <v>4163</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K53" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L53" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N53" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="O53" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="P53" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q53" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="R53" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T53" s="7">
+        <v>1</v>
+      </c>
+      <c r="U53" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V53" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="W53" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="X53" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y53" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="Z53" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC53" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="AD53" s="7"/>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7"/>
+      <c r="AK53" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2026021432</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="3">
+        <v>3853</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N54" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="P54" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T54" s="3">
+        <v>1</v>
+      </c>
+      <c r="U54" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="W54" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="X54" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z54" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA54" s="3"/>
+      <c r="AB54" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC54" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="AD54" s="3"/>
+      <c r="AE54" s="3"/>
+      <c r="AF54" s="3"/>
+      <c r="AG54" s="3"/>
+      <c r="AH54" s="3"/>
+      <c r="AI54" s="3"/>
+      <c r="AJ54" s="3"/>
+      <c r="AK54" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="7">
+        <v>2026021433</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="7">
+        <v>3853</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L55" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="M55" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="N55" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="O55" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="P55" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q55" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T55" s="7">
+        <v>1</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="W55" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="X55" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="Y55" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z55" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA55" s="7"/>
+      <c r="AB55" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC55" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="AD55" s="7"/>
+      <c r="AE55" s="7"/>
+      <c r="AF55" s="7"/>
+      <c r="AG55" s="7"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="7"/>
+      <c r="AK55" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="3">
+        <v>2026021434</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="3">
+        <v>3853</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="P56" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q56" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S56" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T56" s="3">
+        <v>1</v>
+      </c>
+      <c r="U56" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V56" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="X56" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="Y56" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z56" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC56" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="AD56" s="3"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3"/>
+      <c r="AK56" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="7">
+        <v>2026021439</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="F57" s="7">
+        <v>4528</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L57" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M57" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N57" s="7">
+        <v>2301</v>
+      </c>
+      <c r="O57" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="P57" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q57" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T57" s="7">
+        <v>1</v>
+      </c>
+      <c r="U57" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V57" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="W57" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="X57" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="Y57" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="Z57" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC57" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="AD57" s="7"/>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+      <c r="AG57" s="7"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7"/>
+      <c r="AK57" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:37">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2026021445</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N58" s="3">
+        <v>2301</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="P58" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T58" s="3">
+        <v>1</v>
+      </c>
+      <c r="U58" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V58" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="W58" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="X58" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="Y58" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z58" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC58" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="AD58" s="3"/>
+      <c r="AE58" s="3"/>
+      <c r="AF58" s="3"/>
+      <c r="AG58" s="3"/>
+      <c r="AH58" s="3"/>
+      <c r="AI58" s="3"/>
+      <c r="AJ58" s="3"/>
+      <c r="AK58" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="7">
+        <v>2026021446</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="7">
+        <v>4008</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="K59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L59" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="M59" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="N59" s="7">
+        <v>2501</v>
+      </c>
+      <c r="O59" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="P59" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q59" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T59" s="7">
+        <v>1</v>
+      </c>
+      <c r="U59" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V59" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="W59" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="X59" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="Y59" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z59" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA59" s="7"/>
+      <c r="AB59" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC59" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="AD59" s="7"/>
+      <c r="AE59" s="7"/>
+      <c r="AF59" s="7"/>
+      <c r="AG59" s="7"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="7"/>
+      <c r="AJ59" s="7"/>
+      <c r="AK59" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="3">
+        <v>2026021448</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="N60" s="3">
+        <v>5903</v>
+      </c>
+      <c r="O60" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="P60" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="R60" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T60" s="3">
+        <v>1</v>
+      </c>
+      <c r="U60" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V60" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="W60" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="X60" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="Y60" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z60" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC60" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="AD60" s="3"/>
+      <c r="AE60" s="3"/>
+      <c r="AF60" s="3"/>
+      <c r="AG60" s="3"/>
+      <c r="AH60" s="3"/>
+      <c r="AI60" s="3"/>
+      <c r="AJ60" s="3"/>
+      <c r="AK60" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:37">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" s="7">
+        <v>2026021449</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="F61" s="7">
+        <v>4155</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="J61" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L61" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="N61" s="7">
+        <v>2401</v>
+      </c>
+      <c r="O61" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="P61" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q61" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="R61" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T61" s="7">
+        <v>1</v>
+      </c>
+      <c r="U61" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V61" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="W61" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="X61" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="Y61" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="Z61" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC61" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="AD61" s="7"/>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+      <c r="AG61" s="7"/>
+      <c r="AH61" s="7"/>
+      <c r="AI61" s="7"/>
+      <c r="AJ61" s="7"/>
+      <c r="AK61" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="3">
+        <v>2026021452</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="3">
+        <v>5074</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="O62" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="P62" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q62" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S62" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T62" s="3">
+        <v>1</v>
+      </c>
+      <c r="U62" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V62" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="W62" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="X62" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y62" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="Z62" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC62" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="AD62" s="3"/>
+      <c r="AE62" s="3"/>
+      <c r="AF62" s="3"/>
+      <c r="AG62" s="3"/>
+      <c r="AH62" s="3"/>
+      <c r="AI62" s="3"/>
+      <c r="AJ62" s="3"/>
+      <c r="AK62" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" s="7">
+        <v>2026021482</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7">
+        <v>4163</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="9"/>
+      <c r="Q63" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="R63" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T63" s="7">
+        <v>1</v>
+      </c>
+      <c r="U63" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V63" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="W63" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="X63" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC63" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="AD63" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+      <c r="AH63" s="7"/>
+      <c r="AI63" s="7"/>
+      <c r="AJ63" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK63" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:37">
+      <c r="A64" s="3">
+        <v>62</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" s="3">
+        <v>2026021488</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3">
+        <v>4341</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="10"/>
+      <c r="Q64" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S64" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T64" s="3">
+        <v>1</v>
+      </c>
+      <c r="U64" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V64" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="W64" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="X64" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="Y64" s="3"/>
+      <c r="Z64" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA64" s="3"/>
+      <c r="AB64" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC64" s="10" t="s">
+        <v>540</v>
+      </c>
+      <c r="AD64" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE64" s="3"/>
+      <c r="AF64" s="3"/>
+      <c r="AG64" s="3"/>
+      <c r="AH64" s="3"/>
+      <c r="AI64" s="3"/>
+      <c r="AJ64" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK64" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:37">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2026021497</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7">
+        <v>3380</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="R65" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S65" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T65" s="7">
+        <v>1</v>
+      </c>
+      <c r="U65" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V65" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="W65" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="X65" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC65" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="AD65" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="7"/>
+      <c r="AH65" s="7"/>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK65" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2026021545</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="3">
+        <v>5513</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L66" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N66" s="3">
+        <v>3404</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="P66" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q66" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T66" s="3">
+        <v>1</v>
+      </c>
+      <c r="U66" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V66" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="W66" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="X66" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="Y66" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="Z66" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC66" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="AD66" s="3"/>
+      <c r="AE66" s="3"/>
+      <c r="AF66" s="3"/>
+      <c r="AG66" s="3"/>
+      <c r="AH66" s="3"/>
+      <c r="AI66" s="3"/>
+      <c r="AJ66" s="3"/>
+      <c r="AK66" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:37">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C67" s="7">
+        <v>2026021546</v>
+      </c>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7">
+        <v>4035</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="8"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="9"/>
+      <c r="Q67" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="R67" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S67" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T67" s="7">
+        <v>1</v>
+      </c>
+      <c r="U67" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V67" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="W67" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="X67" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="Y67" s="7"/>
+      <c r="Z67" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA67" s="7"/>
+      <c r="AB67" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC67" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="AD67" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE67" s="7"/>
+      <c r="AF67" s="7"/>
+      <c r="AG67" s="7"/>
+      <c r="AH67" s="7"/>
+      <c r="AI67" s="7"/>
+      <c r="AJ67" s="7"/>
+      <c r="AK67" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="3">
+        <v>2026021562</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3">
+        <v>5357</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T68" s="3">
+        <v>1</v>
+      </c>
+      <c r="U68" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V68" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="W68" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="X68" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC68" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="AD68" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="3"/>
+      <c r="AG68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3"/>
+      <c r="AK68" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C69" s="7">
+        <v>2026021628</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="7">
+        <v>4601</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="J69" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="K69" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L69" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="M69" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="N69" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="O69" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="P69" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="Q69" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="R69" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S69" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T69" s="7">
+        <v>1</v>
+      </c>
+      <c r="U69" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V69" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="W69" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="X69" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="Y69" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="Z69" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC69" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="AD69" s="7"/>
+      <c r="AE69" s="7"/>
+      <c r="AF69" s="7"/>
+      <c r="AG69" s="7"/>
+      <c r="AH69" s="7"/>
+      <c r="AI69" s="7"/>
+      <c r="AJ69" s="7"/>
+      <c r="AK69" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37">
+      <c r="A70" s="3">
+        <v>68</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="3">
+        <v>2026021633</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="3">
+        <v>2380</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="N70" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="P70" s="10" t="s">
+        <v>584</v>
+      </c>
+      <c r="Q70" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="R70" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S70" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T70" s="3">
+        <v>1</v>
+      </c>
+      <c r="U70" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V70" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="W70" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="X70" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="Y70" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="Z70" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA70" s="3"/>
+      <c r="AB70" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC70" s="10" t="s">
+        <v>589</v>
+      </c>
+      <c r="AD70" s="3"/>
+      <c r="AE70" s="3"/>
+      <c r="AF70" s="3"/>
+      <c r="AG70" s="3"/>
+      <c r="AH70" s="3"/>
+      <c r="AI70" s="3"/>
+      <c r="AJ70" s="3"/>
+      <c r="AK70" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:37">
+      <c r="A71" s="7">
+        <v>69</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" s="7">
+        <v>2026021655</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7">
+        <v>3853</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="R71" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S71" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T71" s="7">
+        <v>1</v>
+      </c>
+      <c r="U71" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V71" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="W71" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="X71" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA71" s="7"/>
+      <c r="AB71" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC71" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="AD71" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE71" s="7"/>
+      <c r="AF71" s="7"/>
+      <c r="AG71" s="7"/>
+      <c r="AH71" s="7"/>
+      <c r="AI71" s="7"/>
+      <c r="AJ71" s="7"/>
+      <c r="AK71" s="7"/>
+    </row>
+    <row r="72" spans="1:37">
+      <c r="A72" s="3">
+        <v>70</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="3">
+        <v>2026021660</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3">
+        <v>2380</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="10"/>
+      <c r="Q72" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S72" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T72" s="3">
+        <v>1</v>
+      </c>
+      <c r="U72" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V72" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="W72" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="X72" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="Y72" s="3"/>
+      <c r="Z72" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA72" s="3"/>
+      <c r="AB72" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC72" s="10" t="s">
+        <v>595</v>
+      </c>
+      <c r="AD72" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE72" s="3"/>
+      <c r="AF72" s="3"/>
+      <c r="AG72" s="3"/>
+      <c r="AH72" s="3"/>
+      <c r="AI72" s="3"/>
+      <c r="AJ72" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK72" s="3"/>
+    </row>
+    <row r="73" spans="1:37">
+      <c r="A73" s="7">
+        <v>71</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="7">
+        <v>2026021679</v>
+      </c>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="8"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="R73" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S73" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T73" s="7">
+        <v>1</v>
+      </c>
+      <c r="U73" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V73" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="W73" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="X73" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="Y73" s="7"/>
+      <c r="Z73" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA73" s="7"/>
+      <c r="AB73" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC73" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="AD73" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE73" s="7"/>
+      <c r="AF73" s="7"/>
+      <c r="AG73" s="7"/>
+      <c r="AH73" s="7"/>
+      <c r="AI73" s="7"/>
+      <c r="AJ73" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK73" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:37">
+      <c r="A74" s="3">
+        <v>72</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C74" s="3">
+        <v>2026021692</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3">
+        <v>4601</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="10"/>
+      <c r="Q74" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S74" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T74" s="3">
+        <v>1</v>
+      </c>
+      <c r="U74" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V74" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="W74" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="X74" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="Y74" s="3"/>
+      <c r="Z74" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA74" s="3"/>
+      <c r="AB74" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC74" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="AD74" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE74" s="3"/>
+      <c r="AF74" s="3"/>
+      <c r="AG74" s="3"/>
+      <c r="AH74" s="3"/>
+      <c r="AI74" s="3"/>
+      <c r="AJ74" s="3"/>
+      <c r="AK74" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:37">
+      <c r="A75" s="7">
+        <v>73</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C75" s="7">
+        <v>2026021707</v>
+      </c>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7">
+        <v>2743</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="8"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="8"/>
+      <c r="P75" s="9"/>
+      <c r="Q75" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="R75" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S75" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T75" s="7">
+        <v>1</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V75" s="7" t="s">
+        <v>608</v>
+      </c>
+      <c r="W75" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="X75" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="Y75" s="7"/>
+      <c r="Z75" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC75" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="AD75" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
+      <c r="AG75" s="7"/>
+      <c r="AH75" s="7"/>
+      <c r="AI75" s="7"/>
+      <c r="AJ75" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK75" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:37">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2026021720</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3">
+        <v>4208</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="10"/>
+      <c r="Q76" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S76" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T76" s="3">
+        <v>1</v>
+      </c>
+      <c r="U76" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V76" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="W76" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="X76" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="Y76" s="3"/>
+      <c r="Z76" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA76" s="3"/>
+      <c r="AB76" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC76" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="AD76" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE76" s="3"/>
+      <c r="AF76" s="3"/>
+      <c r="AG76" s="3"/>
+      <c r="AH76" s="3"/>
+      <c r="AI76" s="3"/>
+      <c r="AJ76" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK76" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:37">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C77" s="7">
+        <v>2026021721</v>
+      </c>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="8"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="8"/>
+      <c r="P77" s="8"/>
+      <c r="Q77" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="R77" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S77" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T77" s="7">
+        <v>1</v>
+      </c>
+      <c r="U77" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V77" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="W77" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="X77" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="Y77" s="7"/>
+      <c r="Z77" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC77" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="AD77" s="7"/>
+      <c r="AE77" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF77" s="7"/>
+      <c r="AG77" s="7"/>
+      <c r="AH77" s="7"/>
+      <c r="AI77" s="7"/>
+      <c r="AJ77" s="7"/>
+      <c r="AK77" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02111516
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$77</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$81</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="625">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-10  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="656">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-11  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1947,6 +1947,103 @@
   </si>
   <si>
     <t>閉店撤機完成</t>
+  </si>
+  <si>
+    <t>E4541115021001</t>
+  </si>
+  <si>
+    <t>2026-02-10 17:06:35</t>
+  </si>
+  <si>
+    <t>門市反應TM1熱感發票機(BSC-10)印出來的單據中間都會有一條白線，導致條碼很難刷讀，已嘗試重啟設備+重裝紙捲+簡易清潔仍異常..請台芝到店協助(部分條碼無法正常刷讀)</t>
+  </si>
+  <si>
+    <t>2026-02-10 17:11:42</t>
+  </si>
+  <si>
+    <t>2026-02-11 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-11 14:16:00</t>
+  </si>
+  <si>
+    <t>2026-02-11 21:11:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換下8155003474
+換上8155005465</t>
+  </si>
+  <si>
+    <t>E3458115021101</t>
+  </si>
+  <si>
+    <t>八里龍米店</t>
+  </si>
+  <si>
+    <t>2026-02-11 04:59:21</t>
+  </si>
+  <si>
+    <t>凌晨</t>
+  </si>
+  <si>
+    <t>門市反應MMK熱感機T70II無反應，查看設備閃紅燈，已嘗試重啟設備+重裝紙捲仍異常....請台芝到店協助(熱感紙只能印一張，第二張以上印不出來，有時候連第一張也印不出來，故障了)</t>
+  </si>
+  <si>
+    <t>THILF03458</t>
+  </si>
+  <si>
+    <t>2026-02-11 08:55:06</t>
+  </si>
+  <si>
+    <t>2026-02-11 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-11 10:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-12 12:55:00</t>
+  </si>
+  <si>
+    <t>更換出單機
+換下8138001526
+換上8138002965</t>
+  </si>
+  <si>
+    <t>板橋民治店</t>
+  </si>
+  <si>
+    <t>THILF03965</t>
+  </si>
+  <si>
+    <t>2026-02-11 10:50:34</t>
+  </si>
+  <si>
+    <t>2026-02-11 10:35:00</t>
+  </si>
+  <si>
+    <t>2026-02-11 10:47:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002854</t>
+  </si>
+  <si>
+    <t>板橋仁化店</t>
+  </si>
+  <si>
+    <t>THILF03962</t>
+  </si>
+  <si>
+    <t>2026-02-11 11:49:51</t>
+  </si>
+  <si>
+    <t>2026-02-11 10:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-11 11:03:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002853</t>
   </si>
 </sst>
 </file>
@@ -2360,10 +2457,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK77"/>
+  <dimension ref="A1:AK81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A77" sqref="A77"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8895,7 +8992,7 @@
       <c r="M77" s="8"/>
       <c r="N77" s="7"/>
       <c r="O77" s="8"/>
-      <c r="P77" s="8"/>
+      <c r="P77" s="9"/>
       <c r="Q77" s="7" t="s">
         <v>621</v>
       </c>
@@ -8928,7 +9025,7 @@
       <c r="AB77" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC77" s="8" t="s">
+      <c r="AC77" s="9" t="s">
         <v>624</v>
       </c>
       <c r="AD77" s="7"/>
@@ -8941,6 +9038,354 @@
       <c r="AI77" s="7"/>
       <c r="AJ77" s="7"/>
       <c r="AK77" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:37">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" s="3">
+        <v>2026021771</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F78" s="3">
+        <v>4541</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N78" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="P78" s="10" t="s">
+        <v>627</v>
+      </c>
+      <c r="Q78" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S78" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T78" s="3">
+        <v>1</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V78" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="X78" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="Y78" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="Z78" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA78" s="3"/>
+      <c r="AB78" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC78" s="10" t="s">
+        <v>632</v>
+      </c>
+      <c r="AD78" s="3"/>
+      <c r="AE78" s="3"/>
+      <c r="AF78" s="3"/>
+      <c r="AG78" s="3"/>
+      <c r="AH78" s="3"/>
+      <c r="AI78" s="3"/>
+      <c r="AJ78" s="3"/>
+      <c r="AK78" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:37">
+      <c r="A79" s="7">
+        <v>77</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" s="7">
+        <v>2026021793</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F79" s="7">
+        <v>3458</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="J79" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K79" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="L79" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="M79" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="N79" s="7">
+        <v>5903</v>
+      </c>
+      <c r="O79" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="P79" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="Q79" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="R79" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S79" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T79" s="7">
+        <v>1</v>
+      </c>
+      <c r="U79" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V79" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="W79" s="7" t="s">
+        <v>640</v>
+      </c>
+      <c r="X79" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="Y79" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="Z79" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC79" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="AD79" s="7"/>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="7"/>
+      <c r="AG79" s="7"/>
+      <c r="AH79" s="7"/>
+      <c r="AI79" s="7"/>
+      <c r="AJ79" s="7"/>
+      <c r="AK79" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:37">
+      <c r="A80" s="3">
+        <v>78</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" s="3">
+        <v>2026021826</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3">
+        <v>3965</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="10"/>
+      <c r="Q80" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="R80" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S80" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T80" s="3">
+        <v>1</v>
+      </c>
+      <c r="U80" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V80" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="W80" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="X80" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="Y80" s="3"/>
+      <c r="Z80" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="AA80" s="3"/>
+      <c r="AB80" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC80" s="10" t="s">
+        <v>649</v>
+      </c>
+      <c r="AD80" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="3"/>
+      <c r="AG80" s="3"/>
+      <c r="AH80" s="3"/>
+      <c r="AI80" s="3"/>
+      <c r="AJ80" s="3"/>
+      <c r="AK80" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:37">
+      <c r="A81" s="7">
+        <v>79</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C81" s="7">
+        <v>2026021899</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7">
+        <v>3962</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="8"/>
+      <c r="Q81" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="R81" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S81" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T81" s="7">
+        <v>1</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V81" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="W81" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="X81" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC81" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="AD81" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="7"/>
+      <c r="AJ81" s="7"/>
+      <c r="AK81" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02121731
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="656">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-11  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="676">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-12  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2044,6 +2044,67 @@
   </si>
   <si>
     <t>PMQ1+7210002853</t>
+  </si>
+  <si>
+    <t>E3957115021201</t>
+  </si>
+  <si>
+    <t>三重福仁店</t>
+  </si>
+  <si>
+    <t>2026-02-12 08:45:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM2抽屜(外觀顏色:白色，鎖頭置中，編號5001)抽屜彈出時都會卡住有彈出聲彈出一點仍需手動拉出，確認抽屜無卡異物，請台芝到店協助(機台2抽屜彈不太出來)
+ </t>
+  </si>
+  <si>
+    <t>THILF03957</t>
+  </si>
+  <si>
+    <t>2026-02-12 09:07:56</t>
+  </si>
+  <si>
+    <t>2026-02-12 13:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-12 13:45:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 13:07:00</t>
+  </si>
+  <si>
+    <t>更換抽屜導輪.測試正常</t>
+  </si>
+  <si>
+    <t>2026-02-12 14:29:11</t>
+  </si>
+  <si>
+    <t>2026-02-12 13:05:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002783</t>
+  </si>
+  <si>
+    <t>2026-02-12 17:13:31</t>
+  </si>
+  <si>
+    <t>2026-02-12 16:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-12 16:40:00</t>
+  </si>
+  <si>
+    <t>+L90</t>
+  </si>
+  <si>
+    <t>2026-02-12 17:17:32</t>
+  </si>
+  <si>
+    <t>2026-02-12 16:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-12 17:05:00</t>
   </si>
 </sst>
 </file>
@@ -2457,10 +2518,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK81"/>
+  <dimension ref="A1:AK85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A81" sqref="A81"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9340,7 +9401,7 @@
       <c r="M81" s="8"/>
       <c r="N81" s="7"/>
       <c r="O81" s="8"/>
-      <c r="P81" s="8"/>
+      <c r="P81" s="9"/>
       <c r="Q81" s="7" t="s">
         <v>651</v>
       </c>
@@ -9373,7 +9434,7 @@
       <c r="AB81" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC81" s="8" t="s">
+      <c r="AC81" s="9" t="s">
         <v>655</v>
       </c>
       <c r="AD81" s="7" t="s">
@@ -9386,6 +9447,336 @@
       <c r="AI81" s="7"/>
       <c r="AJ81" s="7"/>
       <c r="AK81" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:37">
+      <c r="A82" s="3">
+        <v>80</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="3">
+        <v>2026022074</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F82" s="3">
+        <v>3957</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="K82" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N82" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O82" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P82" s="10" t="s">
+        <v>659</v>
+      </c>
+      <c r="Q82" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="R82" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S82" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T82" s="3">
+        <v>1</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V82" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="X82" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="Y82" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="Z82" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA82" s="3"/>
+      <c r="AB82" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC82" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="AD82" s="3"/>
+      <c r="AE82" s="3"/>
+      <c r="AF82" s="3"/>
+      <c r="AG82" s="3"/>
+      <c r="AH82" s="3"/>
+      <c r="AI82" s="3"/>
+      <c r="AJ82" s="3"/>
+      <c r="AK82" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37">
+      <c r="A83" s="7">
+        <v>81</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2026022176</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7">
+        <v>3957</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="R83" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S83" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T83" s="7">
+        <v>1</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V83" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="W83" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="X83" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC83" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD83" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="7"/>
+      <c r="AG83" s="7"/>
+      <c r="AH83" s="7"/>
+      <c r="AI83" s="7"/>
+      <c r="AJ83" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK83" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:37">
+      <c r="A84" s="3">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C84" s="3">
+        <v>2026022231</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3">
+        <v>4770</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="R84" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T84" s="3">
+        <v>1</v>
+      </c>
+      <c r="U84" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V84" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="X84" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="Y84" s="3"/>
+      <c r="Z84" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA84" s="3"/>
+      <c r="AB84" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC84" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="AD84" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE84" s="3"/>
+      <c r="AF84" s="3"/>
+      <c r="AG84" s="3"/>
+      <c r="AH84" s="3"/>
+      <c r="AI84" s="3"/>
+      <c r="AJ84" s="3"/>
+      <c r="AK84" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="1:37">
+      <c r="A85" s="7">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" s="7">
+        <v>2026022232</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7">
+        <v>4573</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="8"/>
+      <c r="Q85" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="R85" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S85" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T85" s="7">
+        <v>1</v>
+      </c>
+      <c r="U85" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V85" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="W85" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="X85" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="Y85" s="7"/>
+      <c r="Z85" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC85" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="AD85" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
+      <c r="AG85" s="7"/>
+      <c r="AH85" s="7"/>
+      <c r="AI85" s="7"/>
+      <c r="AJ85" s="7"/>
+      <c r="AK85" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02131447
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$99</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="676">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-12  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="754">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-13  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2086,6 +2086,48 @@
     <t>PMQ1+7210002783</t>
   </si>
   <si>
+    <t>E5496115021201</t>
+  </si>
+  <si>
+    <t>新北市民廣場</t>
+  </si>
+  <si>
+    <t>2026-02-12 14:56:16</t>
+  </si>
+  <si>
+    <t>HLL5</t>
+  </si>
+  <si>
+    <t>HL-多卡機TS2000</t>
+  </si>
+  <si>
+    <t>L503</t>
+  </si>
+  <si>
+    <t>門市反應MMK多卡機(TS2000)無法感應讀取悠遊卡，因消費者離開門市未看到錯誤訊息，已有重啟MMK後點選生活&gt;門職專區&gt;讀卡機測試畫面停留至請稍後當機無法下一個步驟再次重啟仍異常...請台芝到店協助(靠卡感應異常)
+02/12  15:04  請門市關機休息，稍晚聯繫...廖</t>
+  </si>
+  <si>
+    <t>THILF05496</t>
+  </si>
+  <si>
+    <t>2026-02-12 15:19:43</t>
+  </si>
+  <si>
+    <t>2026-02-13 12:29:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 12:48:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 19:19:00</t>
+  </si>
+  <si>
+    <t>更換TS2000
+換上：8184001651
+換下：8184001680</t>
+  </si>
+  <si>
     <t>2026-02-12 17:13:31</t>
   </si>
   <si>
@@ -2105,6 +2147,202 @@
   </si>
   <si>
     <t>2026-02-12 17:05:00</t>
+  </si>
+  <si>
+    <t>中和壽南店</t>
+  </si>
+  <si>
+    <t>THILF05401</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:07:10</t>
+  </si>
+  <si>
+    <t>2026-02-13 09:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 09:50:00</t>
+  </si>
+  <si>
+    <t>新莊福祐店</t>
+  </si>
+  <si>
+    <t>THILF03999</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:23:25</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003058</t>
+  </si>
+  <si>
+    <t>新莊巷口店</t>
+  </si>
+  <si>
+    <t>THILF04762</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:38:56</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:45:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003067</t>
+  </si>
+  <si>
+    <t>永和貞寧店</t>
+  </si>
+  <si>
+    <t>THILF03968</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:39:33</t>
+  </si>
+  <si>
+    <t>2026-02-13 09:40:00</t>
+  </si>
+  <si>
+    <t>永和永霖店</t>
+  </si>
+  <si>
+    <t>THILF04019</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:53:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:30:00</t>
+  </si>
+  <si>
+    <t>永和福和花園</t>
+  </si>
+  <si>
+    <t>THILF03082</t>
+  </si>
+  <si>
+    <t>2026-02-13 11:24:20</t>
+  </si>
+  <si>
+    <t>2026-02-13 10:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 11:00:00</t>
+  </si>
+  <si>
+    <t>中和景德店</t>
+  </si>
+  <si>
+    <t>THILF04536</t>
+  </si>
+  <si>
+    <t>2026-02-13 11:50:37</t>
+  </si>
+  <si>
+    <t>2026-02-13 11:07:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 11:27:00</t>
+  </si>
+  <si>
+    <t>蘆洲鷺江店</t>
+  </si>
+  <si>
+    <t>THILF02890</t>
+  </si>
+  <si>
+    <t>2026-02-13 13:58:21</t>
+  </si>
+  <si>
+    <t>2026-02-13 13:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 13:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003074</t>
+  </si>
+  <si>
+    <t>中和和大店</t>
+  </si>
+  <si>
+    <t>THILF02911</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:09:25</t>
+  </si>
+  <si>
+    <t>2026-02-13 13:08:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 13:28:00</t>
+  </si>
+  <si>
+    <t>蘆洲信義店</t>
+  </si>
+  <si>
+    <t>THILF03452</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:10:29</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003076</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:22:51</t>
+  </si>
+  <si>
+    <t>2026-02-13 13:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:00:00</t>
+  </si>
+  <si>
+    <t>蘆洲中山一</t>
+  </si>
+  <si>
+    <t>THILF03929</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:28:43</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:30:00</t>
+  </si>
+  <si>
+    <t>已與店長確認保險櫃只有一個
+PMQ1+7210003078</t>
+  </si>
+  <si>
+    <t>C660</t>
+  </si>
+  <si>
+    <t>中和永安市場</t>
+  </si>
+  <si>
+    <t>THILF0C660</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:33:12</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:32:00</t>
   </si>
 </sst>
 </file>
@@ -2518,10 +2756,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK85"/>
+  <dimension ref="A1:AK99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A85" sqref="A85"/>
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9631,38 +9869,58 @@
         <v>82</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C84" s="3">
-        <v>2026022231</v>
-      </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
+        <v>2026022197</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F84" s="3">
-        <v>4770</v>
+        <v>5496</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>138</v>
+        <v>670</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="10"/>
+        <v>244</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="M84" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="N84" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="O84" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P84" s="10" t="s">
+        <v>675</v>
+      </c>
       <c r="Q84" s="3" t="s">
-        <v>144</v>
+        <v>676</v>
       </c>
       <c r="R84" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S84" s="3" t="s">
-        <v>53</v>
+        <v>251</v>
       </c>
       <c r="T84" s="3">
         <v>1</v>
@@ -9671,15 +9929,17 @@
         <v>54</v>
       </c>
       <c r="V84" s="3" t="s">
-        <v>669</v>
+        <v>677</v>
       </c>
       <c r="W84" s="3" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="X84" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="Y84" s="3"/>
+        <v>679</v>
+      </c>
+      <c r="Y84" s="3" t="s">
+        <v>680</v>
+      </c>
       <c r="Z84" s="3">
         <v>0.3</v>
       </c>
@@ -9688,11 +9948,9 @@
         <v>59</v>
       </c>
       <c r="AC84" s="10" t="s">
-        <v>672</v>
-      </c>
-      <c r="AD84" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>681</v>
+      </c>
+      <c r="AD84" s="3"/>
       <c r="AE84" s="3"/>
       <c r="AF84" s="3"/>
       <c r="AG84" s="3"/>
@@ -9711,15 +9969,15 @@
         <v>115</v>
       </c>
       <c r="C85" s="7">
-        <v>2026022232</v>
+        <v>2026022231</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7">
-        <v>4573</v>
+        <v>4770</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="H85" s="7" t="s">
         <v>65</v>
@@ -9731,9 +9989,9 @@
       <c r="M85" s="8"/>
       <c r="N85" s="7"/>
       <c r="O85" s="8"/>
-      <c r="P85" s="8"/>
+      <c r="P85" s="9"/>
       <c r="Q85" s="7" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="R85" s="7" t="s">
         <v>52</v>
@@ -9748,13 +10006,13 @@
         <v>54</v>
       </c>
       <c r="V85" s="7" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="W85" s="7" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="X85" s="7" t="s">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="Y85" s="7"/>
       <c r="Z85" s="7">
@@ -9764,8 +10022,8 @@
       <c r="AB85" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC85" s="8" t="s">
-        <v>672</v>
+      <c r="AC85" s="9" t="s">
+        <v>685</v>
       </c>
       <c r="AD85" s="7" t="s">
         <v>61</v>
@@ -9777,6 +10035,1094 @@
       <c r="AI85" s="7"/>
       <c r="AJ85" s="7"/>
       <c r="AK85" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:37">
+      <c r="A86" s="3">
+        <v>84</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C86" s="3">
+        <v>2026022232</v>
+      </c>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3">
+        <v>4573</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="10"/>
+      <c r="Q86" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="R86" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S86" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T86" s="3">
+        <v>1</v>
+      </c>
+      <c r="U86" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V86" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="W86" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="X86" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA86" s="3"/>
+      <c r="AB86" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC86" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD86" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="3"/>
+      <c r="AG86" s="3"/>
+      <c r="AH86" s="3"/>
+      <c r="AI86" s="3"/>
+      <c r="AJ86" s="3"/>
+      <c r="AK86" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:37">
+      <c r="A87" s="7">
+        <v>85</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C87" s="7">
+        <v>2026022288</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7">
+        <v>5401</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>689</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="8"/>
+      <c r="N87" s="7"/>
+      <c r="O87" s="8"/>
+      <c r="P87" s="9"/>
+      <c r="Q87" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="R87" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S87" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T87" s="7">
+        <v>1</v>
+      </c>
+      <c r="U87" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V87" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="W87" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="X87" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="Y87" s="7"/>
+      <c r="Z87" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA87" s="7"/>
+      <c r="AB87" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC87" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD87" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE87" s="7"/>
+      <c r="AF87" s="7"/>
+      <c r="AG87" s="7"/>
+      <c r="AH87" s="7"/>
+      <c r="AI87" s="7"/>
+      <c r="AJ87" s="7"/>
+      <c r="AK87" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="1:37">
+      <c r="A88" s="3">
+        <v>86</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C88" s="3">
+        <v>2026022297</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3">
+        <v>3999</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S88" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T88" s="3">
+        <v>1</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V88" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="W88" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="X88" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="Y88" s="3"/>
+      <c r="Z88" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA88" s="3"/>
+      <c r="AB88" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC88" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="AD88" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE88" s="3"/>
+      <c r="AF88" s="3"/>
+      <c r="AG88" s="3"/>
+      <c r="AH88" s="3"/>
+      <c r="AI88" s="3"/>
+      <c r="AJ88" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK88" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:37">
+      <c r="A89" s="7">
+        <v>87</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" s="7">
+        <v>2026022307</v>
+      </c>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7">
+        <v>4762</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I89" s="7"/>
+      <c r="J89" s="7"/>
+      <c r="K89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="8"/>
+      <c r="N89" s="7"/>
+      <c r="O89" s="8"/>
+      <c r="P89" s="9"/>
+      <c r="Q89" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="R89" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T89" s="7">
+        <v>1</v>
+      </c>
+      <c r="U89" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V89" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="W89" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="X89" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="Y89" s="7"/>
+      <c r="Z89" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC89" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="AD89" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE89" s="7"/>
+      <c r="AF89" s="7"/>
+      <c r="AG89" s="7"/>
+      <c r="AH89" s="7"/>
+      <c r="AI89" s="7"/>
+      <c r="AJ89" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK89" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="90" spans="1:37">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2026022308</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3">
+        <v>3968</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="4"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="4"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T90" s="3">
+        <v>1</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="Y90" s="3"/>
+      <c r="Z90" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD90" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+      <c r="AJ90" s="3"/>
+      <c r="AK90" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2026022319</v>
+      </c>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7">
+        <v>4019</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>710</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="R91" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T91" s="7">
+        <v>1</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V91" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="W91" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="X91" s="7" t="s">
+        <v>714</v>
+      </c>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC91" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD91" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7"/>
+      <c r="AK91" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:37">
+      <c r="A92" s="3">
+        <v>90</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2026022329</v>
+      </c>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3">
+        <v>3082</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="4"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="4"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T92" s="3">
+        <v>1</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V92" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="X92" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="Y92" s="3"/>
+      <c r="Z92" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC92" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD92" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE92" s="3"/>
+      <c r="AF92" s="3"/>
+      <c r="AG92" s="3"/>
+      <c r="AH92" s="3"/>
+      <c r="AI92" s="3"/>
+      <c r="AJ92" s="3"/>
+      <c r="AK92" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:37">
+      <c r="A93" s="7">
+        <v>91</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C93" s="7">
+        <v>2026022347</v>
+      </c>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7">
+        <v>4536</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I93" s="7"/>
+      <c r="J93" s="7"/>
+      <c r="K93" s="7"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="8"/>
+      <c r="N93" s="7"/>
+      <c r="O93" s="8"/>
+      <c r="P93" s="9"/>
+      <c r="Q93" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="R93" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S93" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T93" s="7">
+        <v>1</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V93" s="7" t="s">
+        <v>722</v>
+      </c>
+      <c r="W93" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="X93" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="Y93" s="7"/>
+      <c r="Z93" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC93" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD93" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="7"/>
+      <c r="AG93" s="7"/>
+      <c r="AH93" s="7"/>
+      <c r="AI93" s="7"/>
+      <c r="AJ93" s="7"/>
+      <c r="AK93" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:37">
+      <c r="A94" s="3">
+        <v>92</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C94" s="3">
+        <v>2026022352</v>
+      </c>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3">
+        <v>2890</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="10"/>
+      <c r="Q94" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="R94" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S94" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T94" s="3">
+        <v>1</v>
+      </c>
+      <c r="U94" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V94" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="W94" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="X94" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="Y94" s="3"/>
+      <c r="Z94" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA94" s="3"/>
+      <c r="AB94" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC94" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="AD94" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE94" s="3"/>
+      <c r="AF94" s="3"/>
+      <c r="AG94" s="3"/>
+      <c r="AH94" s="3"/>
+      <c r="AI94" s="3"/>
+      <c r="AJ94" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK94" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:37">
+      <c r="A95" s="7">
+        <v>93</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C95" s="7">
+        <v>2026022361</v>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7">
+        <v>2911</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>731</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I95" s="7"/>
+      <c r="J95" s="7"/>
+      <c r="K95" s="7"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="7"/>
+      <c r="O95" s="8"/>
+      <c r="P95" s="9"/>
+      <c r="Q95" s="7" t="s">
+        <v>732</v>
+      </c>
+      <c r="R95" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S95" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T95" s="7">
+        <v>1</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V95" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="W95" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="X95" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="Y95" s="7"/>
+      <c r="Z95" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA95" s="7"/>
+      <c r="AB95" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC95" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD95" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE95" s="7"/>
+      <c r="AF95" s="7"/>
+      <c r="AG95" s="7"/>
+      <c r="AH95" s="7"/>
+      <c r="AI95" s="7"/>
+      <c r="AJ95" s="7"/>
+      <c r="AK95" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="1:37">
+      <c r="A96" s="3">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2026022362</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3">
+        <v>3452</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="R96" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S96" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T96" s="3">
+        <v>1</v>
+      </c>
+      <c r="U96" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V96" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="W96" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="X96" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="Y96" s="3"/>
+      <c r="Z96" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA96" s="3"/>
+      <c r="AB96" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC96" s="10" t="s">
+        <v>740</v>
+      </c>
+      <c r="AD96" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE96" s="3"/>
+      <c r="AF96" s="3"/>
+      <c r="AG96" s="3"/>
+      <c r="AH96" s="3"/>
+      <c r="AI96" s="3"/>
+      <c r="AJ96" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK96" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:37">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C97" s="7">
+        <v>2026022365</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I97" s="7"/>
+      <c r="J97" s="7"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="7"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="7"/>
+      <c r="O97" s="8"/>
+      <c r="P97" s="9"/>
+      <c r="Q97" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="R97" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S97" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T97" s="7">
+        <v>1</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V97" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="W97" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="X97" s="7" t="s">
+        <v>743</v>
+      </c>
+      <c r="Y97" s="7"/>
+      <c r="Z97" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC97" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD97" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE97" s="7"/>
+      <c r="AF97" s="7"/>
+      <c r="AG97" s="7"/>
+      <c r="AH97" s="7"/>
+      <c r="AI97" s="7"/>
+      <c r="AJ97" s="7"/>
+      <c r="AK97" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:37">
+      <c r="A98" s="3">
+        <v>96</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C98" s="3">
+        <v>2026022367</v>
+      </c>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3">
+        <v>3929</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I98" s="3"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="3"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="R98" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T98" s="3">
+        <v>1</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V98" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="W98" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="X98" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="Y98" s="3"/>
+      <c r="Z98" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA98" s="3"/>
+      <c r="AB98" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC98" s="10" t="s">
+        <v>748</v>
+      </c>
+      <c r="AD98" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE98" s="3"/>
+      <c r="AF98" s="3"/>
+      <c r="AG98" s="3"/>
+      <c r="AH98" s="3"/>
+      <c r="AI98" s="3"/>
+      <c r="AJ98" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK98" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:37">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" s="7">
+        <v>2026022368</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="7"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="7"/>
+      <c r="O99" s="8"/>
+      <c r="P99" s="8"/>
+      <c r="Q99" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S99" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T99" s="7">
+        <v>1</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V99" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="W99" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="Y99" s="7"/>
+      <c r="Z99" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA99" s="7"/>
+      <c r="AB99" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC99" s="8" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD99" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE99" s="7"/>
+      <c r="AF99" s="7"/>
+      <c r="AG99" s="7"/>
+      <c r="AH99" s="7"/>
+      <c r="AI99" s="7"/>
+      <c r="AJ99" s="7"/>
+      <c r="AK99" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02241316
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$99</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$122</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="754">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-13  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="914">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-24  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2343,6 +2343,498 @@
   </si>
   <si>
     <t>2026-02-13 14:32:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 15:28:34</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:38:00</t>
+  </si>
+  <si>
+    <t>2026-02-13 14:57:00</t>
+  </si>
+  <si>
+    <t>15364115021501</t>
+  </si>
+  <si>
+    <t>林口舊街店</t>
+  </si>
+  <si>
+    <t>2026-02-15 09:17:28</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)未觸控螢幕但有點選螢幕的聲音，游標亂跳客服無法開啟校正程式，重啟TM仍異常，與門市確認螢幕無保護貼、文宣...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05364</t>
+  </si>
+  <si>
+    <t>2026-02-15 09:20:05</t>
+  </si>
+  <si>
+    <t>2026-02-24 09:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 13:00:00</t>
+  </si>
+  <si>
+    <t>觸控矯正，現場無飄移及自動點選的狀況，目前測試正常</t>
+  </si>
+  <si>
+    <t>13751115021901</t>
+  </si>
+  <si>
+    <t>淡水真理大</t>
+  </si>
+  <si>
+    <t>2026-02-19 10:01:48</t>
+  </si>
+  <si>
+    <t>02/19 10:00啟動緊急叫修:門市SC(SHUTTLE6S)呈現黑底英文畫面，已將電源線拔除休息10分鐘後插回開機仍異常，PING1不通不可VNC
+門市確認帳務做到01/16，暫歇前與通訊健誌副理確認都有收到資料，PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)...還請台芝到店協助處理</t>
+  </si>
+  <si>
+    <t>THILF03751</t>
+  </si>
+  <si>
+    <t>2026-02-19 10:04:51</t>
+  </si>
+  <si>
+    <t>2026-02-19 12:39:00</t>
+  </si>
+  <si>
+    <t>2026-02-19 13:09:00</t>
+  </si>
+  <si>
+    <t>2026-02-19 16:04:00</t>
+  </si>
+  <si>
+    <t>抓不到第一顆硬碟. 更換sata線  即可正常開啟</t>
+  </si>
+  <si>
+    <t>E3853115021901</t>
+  </si>
+  <si>
+    <t>2026-02-19 10:21:10</t>
+  </si>
+  <si>
+    <t>門市反應TM2抽屜(外觀顏色:白色，鎖頭置中，編號無)抽屜彈出時都會卡住有彈出聲彈出一點仍需手動拉出，確認抽屜無卡異物，請台芝到店協助(抽屜卡住)</t>
+  </si>
+  <si>
+    <t>2026-02-19 10:30:58</t>
+  </si>
+  <si>
+    <t>2026-02-24 09:38:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:08:00</t>
+  </si>
+  <si>
+    <t>彈簧軌道調整後測試正常</t>
+  </si>
+  <si>
+    <t>14845115022102</t>
+  </si>
+  <si>
+    <t>2026-02-21 12:40:48</t>
+  </si>
+  <si>
+    <t>門市反應TM2掃描槍(HC76TR)經常刷讀無反應，確認有亮燈有逼聲、鼠標有在輸入位置，已執行掃槍校正仍異常...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-02-21 12:43:58</t>
+  </si>
+  <si>
+    <t>2026-02-22 13:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-22 13:05:00</t>
+  </si>
+  <si>
+    <t>取消叫修</t>
+  </si>
+  <si>
+    <t>取消報修</t>
+  </si>
+  <si>
+    <t>14260115022201</t>
+  </si>
+  <si>
+    <t>三重高中店</t>
+  </si>
+  <si>
+    <t>2026-02-22 09:06:20</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)抽屜無法完全密合，抽屜外觀米白/鑰匙孔右邊/鑰匙孔編號710....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04260</t>
+  </si>
+  <si>
+    <t>2026-02-22 09:13:10</t>
+  </si>
+  <si>
+    <t>2026-02-23 16:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-23 17:10:00</t>
+  </si>
+  <si>
+    <t>彈簧斷裂導致抽屜無法正常關閉</t>
+  </si>
+  <si>
+    <t>1D161115022201</t>
+  </si>
+  <si>
+    <t>D161</t>
+  </si>
+  <si>
+    <t>板橋僑中三</t>
+  </si>
+  <si>
+    <t>2026-02-22 09:34:50</t>
+  </si>
+  <si>
+    <t>不能連線</t>
+  </si>
+  <si>
+    <t>2/22 09:22 啟動緊急叫修：HUB(DES1210-28)-門市反應全店網路不通，含90、91均不通，請門市重啟數據機+HUB+PEPLINK仍異常，請門市查看設備均有正常過電，但門市查看HUB 13PORT有插線有亮燈，將13PORT與1PORT網路線交叉測試，13PORT網路線插在1PORT也有亮燈，1PORT網路線插在13PORT有亮燈，但網路仍異常...須請台芝到店協助確認</t>
+  </si>
+  <si>
+    <t>THILF0D161</t>
+  </si>
+  <si>
+    <t>2026-02-22 09:43:52</t>
+  </si>
+  <si>
+    <t>2026-02-22 12:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-22 14:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-22 15:43:00</t>
+  </si>
+  <si>
+    <t>中華電信數據機出現Alarm亮紅燈，重設Hub無改善此狀況，請騰雲報修中華電信比且請他註解需將橘色網路線插回</t>
+  </si>
+  <si>
+    <t>1D349115022201</t>
+  </si>
+  <si>
+    <t>D349</t>
+  </si>
+  <si>
+    <t>板橋成都店</t>
+  </si>
+  <si>
+    <t>2026-02-22 15:46:47</t>
+  </si>
+  <si>
+    <t>門市反應TM1多卡機(QP3000E)無法使用悠遊卡，已協助操作版更&gt;悠遊卡機重開仍顯示悠遊卡通訊逾時!...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D349</t>
+  </si>
+  <si>
+    <t>2026-02-22 15:49:02</t>
+  </si>
+  <si>
+    <t>2026-02-23 12:55:00</t>
+  </si>
+  <si>
+    <t>2026-02-23 13:25:00</t>
+  </si>
+  <si>
+    <t>14144115022301</t>
+  </si>
+  <si>
+    <t>新莊頭前店</t>
+  </si>
+  <si>
+    <t>2026-02-23 11:10:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應tm1收銀機(TCX800)(抽屜顏色:白色、鑰匙孔位子(中)、鎖頭編號:無編號)抽屜開關會卡卡的，疑似卡榫有問題...請台芝到店協助
+</t>
+  </si>
+  <si>
+    <t>THILF04144</t>
+  </si>
+  <si>
+    <t>2026-02-23 11:11:10</t>
+  </si>
+  <si>
+    <t>2026-02-23 17:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-23 18:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:11:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換上81Z1003807
+換下貼紙無法辨識</t>
+  </si>
+  <si>
+    <t>14144115022302</t>
+  </si>
+  <si>
+    <t>2026-02-23 11:11:19</t>
+  </si>
+  <si>
+    <t>門市反應tm2收銀機(TCX800)(抽屜顏色:白色、鑰匙孔位子(中)、鎖頭編號:無編號)抽屜開關會卡卡的，疑似卡榫有問題...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-02-23 11:11:33</t>
+  </si>
+  <si>
+    <t>2026-02-23 17:00:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換上81Z1003427
+換下81Z1000867</t>
+  </si>
+  <si>
+    <t>1D161115022301</t>
+  </si>
+  <si>
+    <t>2026-02-23 11:01:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB(DES121028)店長昨日反應店內網路不通，今日中華更換數據機，網路有恢復。PING全店僅91不通，請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>2026-02-23 11:18:31</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:19:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:49:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:18:00</t>
+  </si>
+  <si>
+    <t>更換HUB
+換上：8107005258
+換下：8107003709</t>
+  </si>
+  <si>
+    <t>E4208115022301</t>
+  </si>
+  <si>
+    <t>2026-02-23 13:22:20</t>
+  </si>
+  <si>
+    <t>錢匣損壞</t>
+  </si>
+  <si>
+    <t>門市反應tm2(TCX800)抽屜錢匣彈簧損壞2個，抽屜外觀米白/鑰匙孔位置右/鑰匙孔編號709...須請台芝到店協助(TM2錢匣彈簧損壞)</t>
+  </si>
+  <si>
+    <t>2026-02-23 13:36:20</t>
+  </si>
+  <si>
+    <t>2026-02-23 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-23 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 17:36:00</t>
+  </si>
+  <si>
+    <t>調整彈簧</t>
+  </si>
+  <si>
+    <t>八里艾菲爾</t>
+  </si>
+  <si>
+    <t>THILF05466</t>
+  </si>
+  <si>
+    <t>2026-02-23 14:49:15</t>
+  </si>
+  <si>
+    <t>2026-02-23 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-23 14:30:00</t>
+  </si>
+  <si>
+    <t>新開完工已回報0800
+商顯安裝完工
+商顯中華電信安裝
+現場使用中華電信網路
+Peplink已安裝完成</t>
+  </si>
+  <si>
+    <t>2026-02-23 14:49:59</t>
+  </si>
+  <si>
+    <t>新開門市</t>
+  </si>
+  <si>
+    <t>13052115022301</t>
+  </si>
+  <si>
+    <t>2026-02-23 15:06:31</t>
+  </si>
+  <si>
+    <t>HLL7</t>
+  </si>
+  <si>
+    <t>HL-咖啡價目電子看板</t>
+  </si>
+  <si>
+    <t>L702</t>
+  </si>
+  <si>
+    <t>AOC無電源反應(黑屏無畫面)</t>
+  </si>
+  <si>
+    <t>電子看板IOT專線已完成,請派工台芝到店檢測網路</t>
+  </si>
+  <si>
+    <t>2026-02-23 15:17:53</t>
+  </si>
+  <si>
+    <t>2026-02-23 16:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-23 16:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 19:17:00</t>
+  </si>
+  <si>
+    <t>重開商顯 現場測試商顯網路已正常</t>
+  </si>
+  <si>
+    <t>2026-02-23 17:34:43</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002798</t>
+  </si>
+  <si>
+    <t>EC660115022301</t>
+  </si>
+  <si>
+    <t>2026-02-23 20:23:53</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)又觸控不良了，已於2/7進線叫修中心執行觸控校正，當下有好一點點今天一直遲緩或沒反應...需請台芝到店協助(機一觸控不良.麻煩工程師來查修.謝謝)</t>
+  </si>
+  <si>
+    <t>2026-02-23 20:37:31</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:31:00</t>
+  </si>
+  <si>
+    <t>2026-02-25 00:37:00</t>
+  </si>
+  <si>
+    <t>整理排線 清潔螢幕 重新執行校正</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:55:46</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:35:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:50:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002866</t>
+  </si>
+  <si>
+    <t>蘆洲希望店</t>
+  </si>
+  <si>
+    <t>THILF05354</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:58:39</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003089</t>
+  </si>
+  <si>
+    <t>C672</t>
+  </si>
+  <si>
+    <t>中和橋安店</t>
+  </si>
+  <si>
+    <t>THILF0C672</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:26:47</t>
+  </si>
+  <si>
+    <t>2026-02-24 10:45:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:02:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:34:15</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:07:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:24:00</t>
+  </si>
+  <si>
+    <t>中和中板店</t>
+  </si>
+  <si>
+    <t>THILF03569</t>
+  </si>
+  <si>
+    <t>2026-02-24 12:02:31</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:35:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:54:00</t>
+  </si>
+  <si>
+    <t>蘆洲河上洲</t>
+  </si>
+  <si>
+    <t>THILF05430</t>
+  </si>
+  <si>
+    <t>2026-02-24 12:27:07</t>
+  </si>
+  <si>
+    <t>2026-02-24 11:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 12:00:00</t>
   </si>
 </sst>
 </file>
@@ -2756,10 +3248,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK99"/>
+  <dimension ref="A1:AK122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A99" sqref="A99"/>
+      <selection activeCell="AC119" sqref="AC119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11077,7 +11569,7 @@
       <c r="M99" s="8"/>
       <c r="N99" s="7"/>
       <c r="O99" s="8"/>
-      <c r="P99" s="8"/>
+      <c r="P99" s="9"/>
       <c r="Q99" s="7" t="s">
         <v>751</v>
       </c>
@@ -11110,7 +11602,7 @@
       <c r="AB99" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC99" s="8" t="s">
+      <c r="AC99" s="9" t="s">
         <v>685</v>
       </c>
       <c r="AD99" s="7" t="s">
@@ -11123,6 +11615,2039 @@
       <c r="AI99" s="7"/>
       <c r="AJ99" s="7"/>
       <c r="AK99" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="1:37">
+      <c r="A100" s="3">
+        <v>98</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C100" s="3">
+        <v>2026022401</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3">
+        <v>2380</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="R100" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S100" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T100" s="3">
+        <v>1</v>
+      </c>
+      <c r="U100" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V100" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="W100" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="X100" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="Y100" s="3"/>
+      <c r="Z100" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC100" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD100" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="3"/>
+      <c r="AG100" s="3"/>
+      <c r="AH100" s="3"/>
+      <c r="AI100" s="3"/>
+      <c r="AJ100" s="3"/>
+      <c r="AK100" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="101" spans="1:37">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" s="7">
+        <v>2026022436</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101" s="7">
+        <v>5364</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="I101" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="J101" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K101" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L101" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N101" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O101" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="P101" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="Q101" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="R101" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S101" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T101" s="7">
+        <v>1</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V101" s="7" t="s">
+        <v>762</v>
+      </c>
+      <c r="W101" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="Y101" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z101" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC101" s="9" t="s">
+        <v>766</v>
+      </c>
+      <c r="AD101" s="7"/>
+      <c r="AE101" s="7"/>
+      <c r="AF101" s="7"/>
+      <c r="AG101" s="7"/>
+      <c r="AH101" s="7"/>
+      <c r="AI101" s="7"/>
+      <c r="AJ101" s="7"/>
+      <c r="AK101" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:37">
+      <c r="A102" s="3">
+        <v>100</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C102" s="3">
+        <v>2026022460</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>767</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="F102" s="3">
+        <v>3751</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>769</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="M102" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="N102" s="3">
+        <v>2401</v>
+      </c>
+      <c r="O102" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="P102" s="10" t="s">
+        <v>770</v>
+      </c>
+      <c r="Q102" s="3" t="s">
+        <v>771</v>
+      </c>
+      <c r="R102" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S102" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T102" s="3">
+        <v>1</v>
+      </c>
+      <c r="U102" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V102" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="W102" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="X102" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="Y102" s="3" t="s">
+        <v>775</v>
+      </c>
+      <c r="Z102" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC102" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="AD102" s="3"/>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="3"/>
+      <c r="AG102" s="3"/>
+      <c r="AH102" s="3"/>
+      <c r="AI102" s="3"/>
+      <c r="AJ102" s="3"/>
+      <c r="AK102" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:37">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C103" s="7">
+        <v>2026022461</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F103" s="7">
+        <v>3853</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I103" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="J103" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="K103" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L103" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N103" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O103" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P103" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="Q103" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="R103" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T103" s="7">
+        <v>1</v>
+      </c>
+      <c r="U103" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V103" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="W103" s="7" t="s">
+        <v>781</v>
+      </c>
+      <c r="X103" s="7" t="s">
+        <v>782</v>
+      </c>
+      <c r="Y103" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z103" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA103" s="7"/>
+      <c r="AB103" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC103" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="AD103" s="7"/>
+      <c r="AE103" s="7"/>
+      <c r="AF103" s="7"/>
+      <c r="AG103" s="7"/>
+      <c r="AH103" s="7"/>
+      <c r="AI103" s="7"/>
+      <c r="AJ103" s="7"/>
+      <c r="AK103" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:37">
+      <c r="A104" s="3">
+        <v>102</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2026022476</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F104" s="3">
+        <v>4845</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="J104" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="M104" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="N104" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="O104" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="P104" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q104" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="R104" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S104" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T104" s="3">
+        <v>1</v>
+      </c>
+      <c r="U104" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V104" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="W104" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="X104" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="Y104" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z104" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="AC104" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="AD104" s="3"/>
+      <c r="AE104" s="3"/>
+      <c r="AF104" s="3"/>
+      <c r="AG104" s="3"/>
+      <c r="AH104" s="3"/>
+      <c r="AI104" s="3"/>
+      <c r="AJ104" s="3"/>
+      <c r="AK104" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="105" spans="1:37">
+      <c r="A105" s="7">
+        <v>103</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C105" s="7">
+        <v>2026022478</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F105" s="7">
+        <v>4260</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="H105" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I105" s="7" t="s">
+        <v>794</v>
+      </c>
+      <c r="J105" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K105" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L105" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M105" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N105" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O105" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P105" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="Q105" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="R105" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S105" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T105" s="7">
+        <v>1</v>
+      </c>
+      <c r="U105" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V105" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="W105" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="X105" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="Y105" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z105" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA105" s="7"/>
+      <c r="AB105" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC105" s="9" t="s">
+        <v>800</v>
+      </c>
+      <c r="AD105" s="7"/>
+      <c r="AE105" s="7"/>
+      <c r="AF105" s="7"/>
+      <c r="AG105" s="7"/>
+      <c r="AH105" s="7"/>
+      <c r="AI105" s="7"/>
+      <c r="AJ105" s="7"/>
+      <c r="AK105" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="106" spans="1:37">
+      <c r="A106" s="3">
+        <v>104</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C106" s="3">
+        <v>2026022481</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K106" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L106" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M106" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N106" s="3">
+        <v>3402</v>
+      </c>
+      <c r="O106" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="P106" s="10" t="s">
+        <v>806</v>
+      </c>
+      <c r="Q106" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="R106" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S106" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T106" s="3">
+        <v>1</v>
+      </c>
+      <c r="U106" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V106" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="W106" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="X106" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="Y106" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="Z106" s="3">
+        <v>2.2</v>
+      </c>
+      <c r="AA106" s="3"/>
+      <c r="AB106" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC106" s="10" t="s">
+        <v>812</v>
+      </c>
+      <c r="AD106" s="3"/>
+      <c r="AE106" s="3"/>
+      <c r="AF106" s="3"/>
+      <c r="AG106" s="3"/>
+      <c r="AH106" s="3"/>
+      <c r="AI106" s="3"/>
+      <c r="AJ106" s="3"/>
+      <c r="AK106" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:37">
+      <c r="A107" s="7">
+        <v>105</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C107" s="7">
+        <v>2026022491</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="J107" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K107" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L107" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M107" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N107" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O107" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="P107" s="9" t="s">
+        <v>817</v>
+      </c>
+      <c r="Q107" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="R107" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T107" s="7">
+        <v>1</v>
+      </c>
+      <c r="U107" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V107" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="W107" s="7" t="s">
+        <v>820</v>
+      </c>
+      <c r="X107" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="Y107" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="Z107" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA107" s="7"/>
+      <c r="AB107" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="AC107" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="AD107" s="7"/>
+      <c r="AE107" s="7"/>
+      <c r="AF107" s="7"/>
+      <c r="AG107" s="7"/>
+      <c r="AH107" s="7"/>
+      <c r="AI107" s="7"/>
+      <c r="AJ107" s="7"/>
+      <c r="AK107" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:37">
+      <c r="A108" s="3">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="3">
+        <v>2026022530</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F108" s="3">
+        <v>4144</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="H108" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M108" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N108" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O108" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P108" s="10" t="s">
+        <v>825</v>
+      </c>
+      <c r="Q108" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="R108" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S108" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T108" s="3">
+        <v>1</v>
+      </c>
+      <c r="U108" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V108" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="W108" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="X108" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="Y108" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="Z108" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA108" s="3"/>
+      <c r="AB108" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC108" s="10" t="s">
+        <v>831</v>
+      </c>
+      <c r="AD108" s="3"/>
+      <c r="AE108" s="3"/>
+      <c r="AF108" s="3"/>
+      <c r="AG108" s="3"/>
+      <c r="AH108" s="3"/>
+      <c r="AI108" s="3"/>
+      <c r="AJ108" s="3"/>
+      <c r="AK108" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="109" spans="1:37">
+      <c r="A109" s="7">
+        <v>107</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C109" s="7">
+        <v>2026022531</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F109" s="7">
+        <v>4144</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I109" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L109" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M109" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N109" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O109" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P109" s="9" t="s">
+        <v>834</v>
+      </c>
+      <c r="Q109" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="R109" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S109" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T109" s="7">
+        <v>1</v>
+      </c>
+      <c r="U109" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V109" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="W109" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="X109" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="Y109" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="Z109" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA109" s="7"/>
+      <c r="AB109" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC109" s="9" t="s">
+        <v>837</v>
+      </c>
+      <c r="AD109" s="7"/>
+      <c r="AE109" s="7"/>
+      <c r="AF109" s="7"/>
+      <c r="AG109" s="7"/>
+      <c r="AH109" s="7"/>
+      <c r="AI109" s="7"/>
+      <c r="AJ109" s="7"/>
+      <c r="AK109" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:37">
+      <c r="A110" s="3">
+        <v>108</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C110" s="3">
+        <v>2026022538</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N110" s="3">
+        <v>3402</v>
+      </c>
+      <c r="O110" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="P110" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="Q110" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S110" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T110" s="3">
+        <v>1</v>
+      </c>
+      <c r="U110" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="W110" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="X110" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="Y110" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="Z110" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA110" s="3"/>
+      <c r="AB110" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC110" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="AD110" s="3"/>
+      <c r="AE110" s="3"/>
+      <c r="AF110" s="3"/>
+      <c r="AG110" s="3"/>
+      <c r="AH110" s="3"/>
+      <c r="AI110" s="3"/>
+      <c r="AJ110" s="3"/>
+      <c r="AK110" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="111" spans="1:37">
+      <c r="A111" s="7">
+        <v>109</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C111" s="7">
+        <v>2026022585</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F111" s="7">
+        <v>4208</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="H111" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I111" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M111" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N111" s="7">
+        <v>2304</v>
+      </c>
+      <c r="O111" s="8" t="s">
+        <v>848</v>
+      </c>
+      <c r="P111" s="9" t="s">
+        <v>849</v>
+      </c>
+      <c r="Q111" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="R111" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S111" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T111" s="7">
+        <v>1</v>
+      </c>
+      <c r="U111" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V111" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="W111" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="X111" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="Y111" s="7" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z111" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA111" s="7"/>
+      <c r="AB111" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC111" s="9" t="s">
+        <v>854</v>
+      </c>
+      <c r="AD111" s="7"/>
+      <c r="AE111" s="7"/>
+      <c r="AF111" s="7"/>
+      <c r="AG111" s="7"/>
+      <c r="AH111" s="7"/>
+      <c r="AI111" s="7"/>
+      <c r="AJ111" s="7"/>
+      <c r="AK111" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="112" spans="1:37">
+      <c r="A112" s="3">
+        <v>110</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C112" s="3">
+        <v>2026022599</v>
+      </c>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3">
+        <v>5466</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="I112" s="3"/>
+      <c r="J112" s="3"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="10"/>
+      <c r="Q112" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="R112" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S112" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T112" s="3">
+        <v>1</v>
+      </c>
+      <c r="U112" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V112" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="W112" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="X112" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="Y112" s="3"/>
+      <c r="Z112" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="AA112" s="3"/>
+      <c r="AB112" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC112" s="10" t="s">
+        <v>860</v>
+      </c>
+      <c r="AD112" s="3"/>
+      <c r="AE112" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF112" s="3"/>
+      <c r="AG112" s="3"/>
+      <c r="AH112" s="3"/>
+      <c r="AI112" s="3"/>
+      <c r="AJ112" s="3"/>
+      <c r="AK112" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="113" spans="1:37">
+      <c r="A113" s="7">
+        <v>111</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C113" s="7">
+        <v>2026022600</v>
+      </c>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7">
+        <v>5466</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="H113" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="I113" s="7"/>
+      <c r="J113" s="7"/>
+      <c r="K113" s="7"/>
+      <c r="L113" s="7"/>
+      <c r="M113" s="8"/>
+      <c r="N113" s="7"/>
+      <c r="O113" s="8"/>
+      <c r="P113" s="9"/>
+      <c r="Q113" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="R113" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S113" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T113" s="7">
+        <v>1</v>
+      </c>
+      <c r="U113" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V113" s="7" t="s">
+        <v>861</v>
+      </c>
+      <c r="W113" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="X113" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="Y113" s="7"/>
+      <c r="Z113" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="AA113" s="7"/>
+      <c r="AB113" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC113" s="9" t="s">
+        <v>862</v>
+      </c>
+      <c r="AD113" s="7"/>
+      <c r="AE113" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF113" s="7"/>
+      <c r="AG113" s="7"/>
+      <c r="AH113" s="7"/>
+      <c r="AI113" s="7"/>
+      <c r="AJ113" s="7"/>
+      <c r="AK113" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="114" spans="1:37">
+      <c r="A114" s="3">
+        <v>112</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C114" s="3">
+        <v>2026022607</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>863</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F114" s="3">
+        <v>3052</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>865</v>
+      </c>
+      <c r="M114" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="O114" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="P114" s="10" t="s">
+        <v>869</v>
+      </c>
+      <c r="Q114" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S114" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T114" s="3">
+        <v>1</v>
+      </c>
+      <c r="U114" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V114" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="W114" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="X114" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="Y114" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="Z114" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA114" s="3"/>
+      <c r="AB114" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC114" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="AD114" s="3"/>
+      <c r="AE114" s="3"/>
+      <c r="AF114" s="3"/>
+      <c r="AG114" s="3"/>
+      <c r="AH114" s="3"/>
+      <c r="AI114" s="3"/>
+      <c r="AJ114" s="3"/>
+      <c r="AK114" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="115" spans="1:37">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C115" s="7">
+        <v>2026022662</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7">
+        <v>4260</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>793</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="8"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="8"/>
+      <c r="P115" s="9"/>
+      <c r="Q115" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="R115" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T115" s="7">
+        <v>1</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V115" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="W115" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC115" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="AD115" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK115" s="7"/>
+    </row>
+    <row r="116" spans="1:37">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2026022676</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L116" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M116" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N116" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O116" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="P116" s="10" t="s">
+        <v>879</v>
+      </c>
+      <c r="Q116" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T116" s="3">
+        <v>1</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>880</v>
+      </c>
+      <c r="W116" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="X116" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="Y116" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="Z116" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC116" s="10" t="s">
+        <v>884</v>
+      </c>
+      <c r="AD116" s="3"/>
+      <c r="AE116" s="3"/>
+      <c r="AF116" s="3"/>
+      <c r="AG116" s="3"/>
+      <c r="AH116" s="3"/>
+      <c r="AI116" s="3"/>
+      <c r="AJ116" s="3"/>
+      <c r="AK116" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="117" spans="1:37">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C117" s="7">
+        <v>2026022710</v>
+      </c>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="7"/>
+      <c r="O117" s="8"/>
+      <c r="P117" s="9"/>
+      <c r="Q117" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="R117" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V117" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="W117" s="7" t="s">
+        <v>886</v>
+      </c>
+      <c r="X117" s="7" t="s">
+        <v>887</v>
+      </c>
+      <c r="Y117" s="7"/>
+      <c r="Z117" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC117" s="9" t="s">
+        <v>888</v>
+      </c>
+      <c r="AD117" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="7"/>
+      <c r="AH117" s="7"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="7"/>
+      <c r="AK117" s="7"/>
+    </row>
+    <row r="118" spans="1:37">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2026022712</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3">
+        <v>5354</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="3" t="s">
+        <v>890</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T118" s="3">
+        <v>1</v>
+      </c>
+      <c r="U118" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="W118" s="3" t="s">
+        <v>892</v>
+      </c>
+      <c r="X118" s="3" t="s">
+        <v>893</v>
+      </c>
+      <c r="Y118" s="3"/>
+      <c r="Z118" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC118" s="10" t="s">
+        <v>894</v>
+      </c>
+      <c r="AD118" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE118" s="3"/>
+      <c r="AF118" s="3"/>
+      <c r="AG118" s="3"/>
+      <c r="AH118" s="3"/>
+      <c r="AI118" s="3"/>
+      <c r="AJ118" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK118" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" spans="1:37">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C119" s="7">
+        <v>2026022717</v>
+      </c>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7" t="s">
+        <v>895</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>896</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+      <c r="L119" s="7"/>
+      <c r="M119" s="8"/>
+      <c r="N119" s="7"/>
+      <c r="O119" s="8"/>
+      <c r="P119" s="9"/>
+      <c r="Q119" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="R119" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T119" s="7">
+        <v>1</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V119" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="W119" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="X119" s="7" t="s">
+        <v>900</v>
+      </c>
+      <c r="Y119" s="7"/>
+      <c r="Z119" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC119" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD119" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="7"/>
+      <c r="AH119" s="7"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="7"/>
+      <c r="AK119" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:37">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2026022719</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <v>4008</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T120" s="3">
+        <v>1</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="W120" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="X120" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC120" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD120" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE120" s="3"/>
+      <c r="AF120" s="3"/>
+      <c r="AG120" s="3"/>
+      <c r="AH120" s="3"/>
+      <c r="AI120" s="3"/>
+      <c r="AJ120" s="3"/>
+      <c r="AK120" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="1:37">
+      <c r="A121" s="7">
+        <v>119</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C121" s="7">
+        <v>2026022724</v>
+      </c>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7">
+        <v>3569</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H121" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I121" s="7"/>
+      <c r="J121" s="7"/>
+      <c r="K121" s="7"/>
+      <c r="L121" s="7"/>
+      <c r="M121" s="8"/>
+      <c r="N121" s="7"/>
+      <c r="O121" s="8"/>
+      <c r="P121" s="9"/>
+      <c r="Q121" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="R121" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S121" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T121" s="7">
+        <v>1</v>
+      </c>
+      <c r="U121" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V121" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="W121" s="7" t="s">
+        <v>907</v>
+      </c>
+      <c r="X121" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC121" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD121" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="7"/>
+      <c r="AH121" s="7"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="7"/>
+      <c r="AK121" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:37">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2026022726</v>
+      </c>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3">
+        <v>5430</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I122" s="3"/>
+      <c r="J122" s="3"/>
+      <c r="K122" s="3"/>
+      <c r="L122" s="3"/>
+      <c r="M122" s="4"/>
+      <c r="N122" s="3"/>
+      <c r="O122" s="4"/>
+      <c r="P122" s="4"/>
+      <c r="Q122" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T122" s="3">
+        <v>1</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>913</v>
+      </c>
+      <c r="Y122" s="3"/>
+      <c r="Z122" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC122" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD122" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE122" s="3"/>
+      <c r="AF122" s="3"/>
+      <c r="AG122" s="3"/>
+      <c r="AH122" s="3"/>
+      <c r="AI122" s="3"/>
+      <c r="AJ122" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK122" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02250933
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$122</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$130</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="914">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-24  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="969">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-25  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2684,27 +2684,54 @@
     <t>新開門市</t>
   </si>
   <si>
+    <t>15491115022301</t>
+  </si>
+  <si>
+    <t>三重向日葵</t>
+  </si>
+  <si>
+    <t>2026-02-23 15:09:54</t>
+  </si>
+  <si>
+    <t>HLL7</t>
+  </si>
+  <si>
+    <t>HL-咖啡價目電子看板</t>
+  </si>
+  <si>
+    <t>L702</t>
+  </si>
+  <si>
+    <t>AOC無電源反應(黑屏無畫面)</t>
+  </si>
+  <si>
+    <t>電子看板IOT專線已完成,請派工台芝到店檢測網路</t>
+  </si>
+  <si>
+    <t>THILF05491</t>
+  </si>
+  <si>
+    <t>2026-02-23 15:15:57</t>
+  </si>
+  <si>
+    <t>2026-02-24 14:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 14:40:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 19:15:00</t>
+  </si>
+  <si>
+    <t>重開商險 網路測試正常</t>
+  </si>
+  <si>
     <t>13052115022301</t>
   </si>
   <si>
     <t>2026-02-23 15:06:31</t>
   </si>
   <si>
-    <t>HLL7</t>
-  </si>
-  <si>
-    <t>HL-咖啡價目電子看板</t>
-  </si>
-  <si>
-    <t>L702</t>
-  </si>
-  <si>
-    <t>AOC無電源反應(黑屏無畫面)</t>
-  </si>
-  <si>
-    <t>電子看板IOT專線已完成,請派工台芝到店檢測網路</t>
-  </si>
-  <si>
     <t>2026-02-23 15:17:53</t>
   </si>
   <si>
@@ -2720,12 +2747,65 @@
     <t>重開商顯 現場測試商顯網路已正常</t>
   </si>
   <si>
+    <t>15430115022301</t>
+  </si>
+  <si>
+    <t>蘆洲河上洲</t>
+  </si>
+  <si>
+    <t>2026-02-23 15:00:40</t>
+  </si>
+  <si>
+    <t>THILF05430</t>
+  </si>
+  <si>
+    <t>2026-02-23 15:18:08</t>
+  </si>
+  <si>
+    <t>2026-02-24 17:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 17:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 19:18:00</t>
+  </si>
+  <si>
+    <t>到場商顯無網路訊號，後場查無TV線路</t>
+  </si>
+  <si>
     <t>2026-02-23 17:34:43</t>
   </si>
   <si>
     <t>PMQ1+7210002798</t>
   </si>
   <si>
+    <t>14208115022301</t>
+  </si>
+  <si>
+    <t>2026-02-23 18:51:47</t>
+  </si>
+  <si>
+    <t>門市反應TM2熱感發票機(BSC 10)印出的條碼(例:牛奶兌換卷、滿額168兌換卷)於TM1.2皆無法刷讀，已有將發票機關機紙捲重裝與簡易清潔仍異常...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-02-23 18:54:21</t>
+  </si>
+  <si>
+    <t>2026-02-24 16:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 17:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 22:54:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換上8155004420
+換下8155003589</t>
+  </si>
+  <si>
     <t>EC660115022301</t>
   </si>
   <si>
@@ -2822,12 +2902,6 @@
     <t>2026-02-24 11:54:00</t>
   </si>
   <si>
-    <t>蘆洲河上洲</t>
-  </si>
-  <si>
-    <t>THILF05430</t>
-  </si>
-  <si>
     <t>2026-02-24 12:27:07</t>
   </si>
   <si>
@@ -2835,6 +2909,99 @@
   </si>
   <si>
     <t>2026-02-24 12:00:00</t>
+  </si>
+  <si>
+    <t>桃縣桃楚店</t>
+  </si>
+  <si>
+    <t>THILF03045</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:22:58</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:22:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002732+L90</t>
+  </si>
+  <si>
+    <t>三重五常店</t>
+  </si>
+  <si>
+    <t>THILF05316</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:37:13</t>
+  </si>
+  <si>
+    <t>2026-02-24 14:55:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:15:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002811</t>
+  </si>
+  <si>
+    <t>三重進安店</t>
+  </si>
+  <si>
+    <t>THILF03796</t>
+  </si>
+  <si>
+    <t>2026-02-24 16:02:40</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:46:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002779</t>
+  </si>
+  <si>
+    <t>蘆竹海山店</t>
+  </si>
+  <si>
+    <t>THILF04673</t>
+  </si>
+  <si>
+    <t>2026-02-24 16:18:13</t>
+  </si>
+  <si>
+    <t>2026-02-24 15:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 16:17:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002741+L90</t>
+  </si>
+  <si>
+    <t>D194</t>
+  </si>
+  <si>
+    <t>北縣五華三店</t>
+  </si>
+  <si>
+    <t>THILF0D194</t>
+  </si>
+  <si>
+    <t>2026-02-24 16:36:27</t>
+  </si>
+  <si>
+    <t>2026-02-24 16:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-24 16:21:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002821</t>
   </si>
 </sst>
 </file>
@@ -3248,10 +3415,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK122"/>
+  <dimension ref="A1:AK130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC119" sqref="AC119"/>
+      <selection activeCell="AC127" sqref="AC127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12924,7 +13091,7 @@
         <v>38</v>
       </c>
       <c r="C114" s="3">
-        <v>2026022607</v>
+        <v>2026022605</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>863</v>
@@ -12933,16 +13100,16 @@
         <v>40</v>
       </c>
       <c r="F114" s="3">
-        <v>3052</v>
+        <v>5491</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>186</v>
+        <v>864</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>127</v>
+        <v>42</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="J114" s="3" t="s">
         <v>104</v>
@@ -12951,28 +13118,28 @@
         <v>45</v>
       </c>
       <c r="L114" s="3" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="M114" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="N114" s="3" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="O114" s="4" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="P114" s="10" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="Q114" s="3" t="s">
-        <v>194</v>
+        <v>871</v>
       </c>
       <c r="R114" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S114" s="3" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="T114" s="3">
         <v>1</v>
@@ -12981,16 +13148,16 @@
         <v>54</v>
       </c>
       <c r="V114" s="3" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="W114" s="3" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="X114" s="3" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="Y114" s="3" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="Z114" s="3">
         <v>0.5</v>
@@ -13000,7 +13167,7 @@
         <v>59</v>
       </c>
       <c r="AC114" s="10" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="AD114" s="3"/>
       <c r="AE114" s="3"/>
@@ -13018,38 +13185,58 @@
         <v>113</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C115" s="7">
-        <v>2026022662</v>
-      </c>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
+        <v>2026022607</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>877</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F115" s="7">
-        <v>4260</v>
+        <v>3052</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>793</v>
+        <v>186</v>
       </c>
       <c r="H115" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I115" s="7"/>
-      <c r="J115" s="7"/>
-      <c r="K115" s="7"/>
-      <c r="L115" s="7"/>
-      <c r="M115" s="8"/>
-      <c r="N115" s="7"/>
-      <c r="O115" s="8"/>
-      <c r="P115" s="9"/>
+        <v>127</v>
+      </c>
+      <c r="I115" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="J115" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K115" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L115" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="M115" s="8" t="s">
+        <v>867</v>
+      </c>
+      <c r="N115" s="7" t="s">
+        <v>868</v>
+      </c>
+      <c r="O115" s="8" t="s">
+        <v>869</v>
+      </c>
+      <c r="P115" s="9" t="s">
+        <v>870</v>
+      </c>
       <c r="Q115" s="7" t="s">
-        <v>796</v>
+        <v>194</v>
       </c>
       <c r="R115" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S115" s="7" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="T115" s="7">
         <v>1</v>
@@ -13058,37 +13245,37 @@
         <v>54</v>
       </c>
       <c r="V115" s="7" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="W115" s="7" t="s">
-        <v>799</v>
+        <v>880</v>
       </c>
       <c r="X115" s="7" t="s">
-        <v>828</v>
-      </c>
-      <c r="Y115" s="7"/>
+        <v>881</v>
+      </c>
+      <c r="Y115" s="7" t="s">
+        <v>882</v>
+      </c>
       <c r="Z115" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA115" s="7"/>
       <c r="AB115" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC115" s="9" t="s">
-        <v>876</v>
-      </c>
-      <c r="AD115" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>883</v>
+      </c>
+      <c r="AD115" s="7"/>
       <c r="AE115" s="7"/>
       <c r="AF115" s="7"/>
       <c r="AG115" s="7"/>
       <c r="AH115" s="7"/>
       <c r="AI115" s="7"/>
-      <c r="AJ115" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK115" s="7"/>
+      <c r="AJ115" s="7"/>
+      <c r="AK115" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="116" spans="1:37">
       <c r="A116" s="3">
@@ -13098,55 +13285,55 @@
         <v>38</v>
       </c>
       <c r="C116" s="3">
-        <v>2026022676</v>
+        <v>2026022608</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F116" s="3" t="s">
-        <v>749</v>
+      <c r="F116" s="3">
+        <v>5430</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>750</v>
+        <v>885</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>878</v>
+        <v>886</v>
       </c>
       <c r="J116" s="3" t="s">
         <v>104</v>
       </c>
       <c r="K116" s="3" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="L116" s="3" t="s">
-        <v>68</v>
+        <v>866</v>
       </c>
       <c r="M116" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="N116" s="3">
-        <v>2307</v>
+        <v>867</v>
+      </c>
+      <c r="N116" s="3" t="s">
+        <v>868</v>
       </c>
       <c r="O116" s="4" t="s">
-        <v>315</v>
+        <v>869</v>
       </c>
       <c r="P116" s="10" t="s">
-        <v>879</v>
+        <v>870</v>
       </c>
       <c r="Q116" s="3" t="s">
-        <v>751</v>
+        <v>887</v>
       </c>
       <c r="R116" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S116" s="3" t="s">
-        <v>53</v>
+        <v>251</v>
       </c>
       <c r="T116" s="3">
         <v>1</v>
@@ -13155,26 +13342,26 @@
         <v>54</v>
       </c>
       <c r="V116" s="3" t="s">
-        <v>880</v>
+        <v>888</v>
       </c>
       <c r="W116" s="3" t="s">
-        <v>881</v>
+        <v>889</v>
       </c>
       <c r="X116" s="3" t="s">
-        <v>882</v>
+        <v>890</v>
       </c>
       <c r="Y116" s="3" t="s">
-        <v>883</v>
+        <v>891</v>
       </c>
       <c r="Z116" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA116" s="3"/>
       <c r="AB116" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC116" s="10" t="s">
-        <v>884</v>
+        <v>892</v>
       </c>
       <c r="AD116" s="3"/>
       <c r="AE116" s="3"/>
@@ -13195,18 +13382,18 @@
         <v>115</v>
       </c>
       <c r="C117" s="7">
-        <v>2026022710</v>
+        <v>2026022662</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
-      <c r="F117" s="7" t="s">
-        <v>802</v>
+      <c r="F117" s="7">
+        <v>4260</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>803</v>
+        <v>793</v>
       </c>
       <c r="H117" s="7" t="s">
-        <v>244</v>
+        <v>42</v>
       </c>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
@@ -13217,13 +13404,13 @@
       <c r="O117" s="8"/>
       <c r="P117" s="9"/>
       <c r="Q117" s="7" t="s">
-        <v>807</v>
+        <v>796</v>
       </c>
       <c r="R117" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S117" s="7" t="s">
-        <v>251</v>
+        <v>53</v>
       </c>
       <c r="T117" s="7">
         <v>1</v>
@@ -13232,13 +13419,13 @@
         <v>54</v>
       </c>
       <c r="V117" s="7" t="s">
-        <v>885</v>
+        <v>893</v>
       </c>
       <c r="W117" s="7" t="s">
-        <v>886</v>
+        <v>799</v>
       </c>
       <c r="X117" s="7" t="s">
-        <v>887</v>
+        <v>828</v>
       </c>
       <c r="Y117" s="7"/>
       <c r="Z117" s="7">
@@ -13249,7 +13436,7 @@
         <v>59</v>
       </c>
       <c r="AC117" s="9" t="s">
-        <v>888</v>
+        <v>894</v>
       </c>
       <c r="AD117" s="7" t="s">
         <v>61</v>
@@ -13259,7 +13446,9 @@
       <c r="AG117" s="7"/>
       <c r="AH117" s="7"/>
       <c r="AI117" s="7"/>
-      <c r="AJ117" s="7"/>
+      <c r="AJ117" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="AK117" s="7"/>
     </row>
     <row r="118" spans="1:37">
@@ -13267,32 +13456,52 @@
         <v>116</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C118" s="3">
-        <v>2026022712</v>
-      </c>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
+        <v>2026022675</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F118" s="3">
-        <v>5354</v>
+        <v>4208</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>889</v>
+        <v>612</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
-      <c r="K118" s="3"/>
-      <c r="L118" s="3"/>
-      <c r="M118" s="4"/>
-      <c r="N118" s="3"/>
-      <c r="O118" s="4"/>
-      <c r="P118" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K118" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L118" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M118" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N118" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="O118" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="P118" s="10" t="s">
+        <v>897</v>
+      </c>
       <c r="Q118" s="3" t="s">
-        <v>890</v>
+        <v>613</v>
       </c>
       <c r="R118" s="3" t="s">
         <v>52</v>
@@ -13307,36 +13516,34 @@
         <v>54</v>
       </c>
       <c r="V118" s="3" t="s">
-        <v>891</v>
+        <v>898</v>
       </c>
       <c r="W118" s="3" t="s">
-        <v>892</v>
+        <v>899</v>
       </c>
       <c r="X118" s="3" t="s">
-        <v>893</v>
-      </c>
-      <c r="Y118" s="3"/>
+        <v>900</v>
+      </c>
+      <c r="Y118" s="3" t="s">
+        <v>901</v>
+      </c>
       <c r="Z118" s="3">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="AA118" s="3"/>
       <c r="AB118" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC118" s="10" t="s">
-        <v>894</v>
-      </c>
-      <c r="AD118" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>902</v>
+      </c>
+      <c r="AD118" s="3"/>
       <c r="AE118" s="3"/>
       <c r="AF118" s="3"/>
       <c r="AG118" s="3"/>
       <c r="AH118" s="3"/>
       <c r="AI118" s="3"/>
-      <c r="AJ118" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ118" s="3"/>
       <c r="AK118" s="3" t="s">
         <v>61</v>
       </c>
@@ -13346,32 +13553,52 @@
         <v>117</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C119" s="7">
-        <v>2026022717</v>
-      </c>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
+        <v>2026022676</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F119" s="7" t="s">
-        <v>895</v>
+        <v>749</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>896</v>
+        <v>750</v>
       </c>
       <c r="H119" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="I119" s="7"/>
-      <c r="J119" s="7"/>
-      <c r="K119" s="7"/>
-      <c r="L119" s="7"/>
-      <c r="M119" s="8"/>
-      <c r="N119" s="7"/>
-      <c r="O119" s="8"/>
-      <c r="P119" s="9"/>
+      <c r="I119" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K119" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L119" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M119" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N119" s="7">
+        <v>2307</v>
+      </c>
+      <c r="O119" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="P119" s="9" t="s">
+        <v>905</v>
+      </c>
       <c r="Q119" s="7" t="s">
-        <v>897</v>
+        <v>751</v>
       </c>
       <c r="R119" s="7" t="s">
         <v>52</v>
@@ -13386,28 +13613,28 @@
         <v>54</v>
       </c>
       <c r="V119" s="7" t="s">
-        <v>898</v>
+        <v>906</v>
       </c>
       <c r="W119" s="7" t="s">
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="X119" s="7" t="s">
-        <v>900</v>
-      </c>
-      <c r="Y119" s="7"/>
+        <v>908</v>
+      </c>
+      <c r="Y119" s="7" t="s">
+        <v>909</v>
+      </c>
       <c r="Z119" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA119" s="7"/>
       <c r="AB119" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC119" s="9" t="s">
-        <v>685</v>
-      </c>
-      <c r="AD119" s="7" t="s">
-        <v>61</v>
-      </c>
+        <v>910</v>
+      </c>
+      <c r="AD119" s="7"/>
       <c r="AE119" s="7"/>
       <c r="AF119" s="7"/>
       <c r="AG119" s="7"/>
@@ -13426,18 +13653,18 @@
         <v>115</v>
       </c>
       <c r="C120" s="3">
-        <v>2026022719</v>
+        <v>2026022710</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="3">
-        <v>4008</v>
+      <c r="F120" s="3" t="s">
+        <v>802</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>165</v>
+        <v>803</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>65</v>
+        <v>244</v>
       </c>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
@@ -13448,13 +13675,13 @@
       <c r="O120" s="4"/>
       <c r="P120" s="10"/>
       <c r="Q120" s="3" t="s">
-        <v>166</v>
+        <v>807</v>
       </c>
       <c r="R120" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S120" s="3" t="s">
-        <v>53</v>
+        <v>251</v>
       </c>
       <c r="T120" s="3">
         <v>1</v>
@@ -13463,13 +13690,13 @@
         <v>54</v>
       </c>
       <c r="V120" s="3" t="s">
-        <v>901</v>
+        <v>911</v>
       </c>
       <c r="W120" s="3" t="s">
-        <v>902</v>
+        <v>912</v>
       </c>
       <c r="X120" s="3" t="s">
-        <v>903</v>
+        <v>913</v>
       </c>
       <c r="Y120" s="3"/>
       <c r="Z120" s="3">
@@ -13480,7 +13707,7 @@
         <v>59</v>
       </c>
       <c r="AC120" s="10" t="s">
-        <v>685</v>
+        <v>914</v>
       </c>
       <c r="AD120" s="3" t="s">
         <v>61</v>
@@ -13491,9 +13718,7 @@
       <c r="AH120" s="3"/>
       <c r="AI120" s="3"/>
       <c r="AJ120" s="3"/>
-      <c r="AK120" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AK120" s="3"/>
     </row>
     <row r="121" spans="1:37">
       <c r="A121" s="7">
@@ -13503,18 +13728,18 @@
         <v>115</v>
       </c>
       <c r="C121" s="7">
-        <v>2026022724</v>
+        <v>2026022712</v>
       </c>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7">
-        <v>3569</v>
+        <v>5354</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>904</v>
+        <v>915</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
@@ -13525,13 +13750,13 @@
       <c r="O121" s="8"/>
       <c r="P121" s="9"/>
       <c r="Q121" s="7" t="s">
-        <v>905</v>
+        <v>916</v>
       </c>
       <c r="R121" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S121" s="7" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="T121" s="7">
         <v>1</v>
@@ -13540,24 +13765,24 @@
         <v>54</v>
       </c>
       <c r="V121" s="7" t="s">
-        <v>906</v>
+        <v>917</v>
       </c>
       <c r="W121" s="7" t="s">
-        <v>907</v>
+        <v>918</v>
       </c>
       <c r="X121" s="7" t="s">
-        <v>908</v>
+        <v>919</v>
       </c>
       <c r="Y121" s="7"/>
       <c r="Z121" s="7">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA121" s="7"/>
       <c r="AB121" s="7" t="s">
         <v>59</v>
       </c>
       <c r="AC121" s="9" t="s">
-        <v>685</v>
+        <v>920</v>
       </c>
       <c r="AD121" s="7" t="s">
         <v>61</v>
@@ -13567,7 +13792,9 @@
       <c r="AG121" s="7"/>
       <c r="AH121" s="7"/>
       <c r="AI121" s="7"/>
-      <c r="AJ121" s="7"/>
+      <c r="AJ121" s="7" t="s">
+        <v>61</v>
+      </c>
       <c r="AK121" s="7" t="s">
         <v>61</v>
       </c>
@@ -13580,18 +13807,18 @@
         <v>115</v>
       </c>
       <c r="C122" s="3">
-        <v>2026022726</v>
+        <v>2026022717</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="3">
-        <v>5430</v>
+      <c r="F122" s="3" t="s">
+        <v>921</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>909</v>
+        <v>922</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>152</v>
+        <v>65</v>
       </c>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
@@ -13600,15 +13827,15 @@
       <c r="M122" s="4"/>
       <c r="N122" s="3"/>
       <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
+      <c r="P122" s="10"/>
       <c r="Q122" s="3" t="s">
-        <v>910</v>
+        <v>923</v>
       </c>
       <c r="R122" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S122" s="3" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="T122" s="3">
         <v>1</v>
@@ -13617,24 +13844,24 @@
         <v>54</v>
       </c>
       <c r="V122" s="3" t="s">
-        <v>911</v>
+        <v>924</v>
       </c>
       <c r="W122" s="3" t="s">
-        <v>912</v>
+        <v>925</v>
       </c>
       <c r="X122" s="3" t="s">
-        <v>913</v>
+        <v>926</v>
       </c>
       <c r="Y122" s="3"/>
       <c r="Z122" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA122" s="3"/>
       <c r="AB122" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC122" s="4" t="s">
-        <v>118</v>
+      <c r="AC122" s="10" t="s">
+        <v>685</v>
       </c>
       <c r="AD122" s="3" t="s">
         <v>61</v>
@@ -13644,10 +13871,632 @@
       <c r="AG122" s="3"/>
       <c r="AH122" s="3"/>
       <c r="AI122" s="3"/>
-      <c r="AJ122" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AJ122" s="3"/>
       <c r="AK122" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:37">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C123" s="7">
+        <v>2026022719</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7">
+        <v>4008</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="7"/>
+      <c r="O123" s="8"/>
+      <c r="P123" s="9"/>
+      <c r="Q123" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="R123" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T123" s="7">
+        <v>1</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V123" s="7" t="s">
+        <v>927</v>
+      </c>
+      <c r="W123" s="7" t="s">
+        <v>928</v>
+      </c>
+      <c r="X123" s="7" t="s">
+        <v>929</v>
+      </c>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC123" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD123" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE123" s="7"/>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7"/>
+      <c r="AK123" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="124" spans="1:37">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2026022724</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3">
+        <v>3569</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>930</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="3" t="s">
+        <v>931</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T124" s="3">
+        <v>1</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="Y124" s="3"/>
+      <c r="Z124" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC124" s="10" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD124" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE124" s="3"/>
+      <c r="AF124" s="3"/>
+      <c r="AG124" s="3"/>
+      <c r="AH124" s="3"/>
+      <c r="AI124" s="3"/>
+      <c r="AJ124" s="3"/>
+      <c r="AK124" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:37">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2026022726</v>
+      </c>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7">
+        <v>5430</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="I125" s="7"/>
+      <c r="J125" s="7"/>
+      <c r="K125" s="7"/>
+      <c r="L125" s="7"/>
+      <c r="M125" s="8"/>
+      <c r="N125" s="7"/>
+      <c r="O125" s="8"/>
+      <c r="P125" s="9"/>
+      <c r="Q125" s="7" t="s">
+        <v>887</v>
+      </c>
+      <c r="R125" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T125" s="7">
+        <v>1</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V125" s="7" t="s">
+        <v>935</v>
+      </c>
+      <c r="W125" s="7" t="s">
+        <v>936</v>
+      </c>
+      <c r="X125" s="7" t="s">
+        <v>937</v>
+      </c>
+      <c r="Y125" s="7"/>
+      <c r="Z125" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC125" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD125" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="7"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK125" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:37">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2026022786</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3">
+        <v>3045</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="10"/>
+      <c r="Q126" s="3" t="s">
+        <v>939</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T126" s="3">
+        <v>1</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="Y126" s="3"/>
+      <c r="Z126" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA126" s="3"/>
+      <c r="AB126" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC126" s="10" t="s">
+        <v>943</v>
+      </c>
+      <c r="AD126" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE126" s="3"/>
+      <c r="AF126" s="3"/>
+      <c r="AG126" s="3"/>
+      <c r="AH126" s="3"/>
+      <c r="AI126" s="3"/>
+      <c r="AJ126" s="3"/>
+      <c r="AK126" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="127" spans="1:37">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C127" s="7">
+        <v>2026022789</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7">
+        <v>5316</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>944</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="R127" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S127" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T127" s="7">
+        <v>1</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V127" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="W127" s="7" t="s">
+        <v>947</v>
+      </c>
+      <c r="X127" s="7" t="s">
+        <v>948</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>949</v>
+      </c>
+      <c r="AD127" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE127" s="7"/>
+      <c r="AF127" s="7"/>
+      <c r="AG127" s="7"/>
+      <c r="AH127" s="7"/>
+      <c r="AI127" s="7"/>
+      <c r="AJ127" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK127" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="128" spans="1:37">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2026022810</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3">
+        <v>3796</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I128" s="3"/>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="3"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="3"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="10"/>
+      <c r="Q128" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T128" s="3">
+        <v>1</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="W128" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="X128" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="Y128" s="3"/>
+      <c r="Z128" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA128" s="3"/>
+      <c r="AB128" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC128" s="10" t="s">
+        <v>955</v>
+      </c>
+      <c r="AD128" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE128" s="3"/>
+      <c r="AF128" s="3"/>
+      <c r="AG128" s="3"/>
+      <c r="AH128" s="3"/>
+      <c r="AI128" s="3"/>
+      <c r="AJ128" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK128" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="129" spans="1:37">
+      <c r="A129" s="7">
+        <v>127</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C129" s="7">
+        <v>2026022812</v>
+      </c>
+      <c r="D129" s="7"/>
+      <c r="E129" s="7"/>
+      <c r="F129" s="7">
+        <v>4673</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+      <c r="K129" s="7"/>
+      <c r="L129" s="7"/>
+      <c r="M129" s="8"/>
+      <c r="N129" s="7"/>
+      <c r="O129" s="8"/>
+      <c r="P129" s="9"/>
+      <c r="Q129" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="R129" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S129" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T129" s="7">
+        <v>1</v>
+      </c>
+      <c r="U129" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V129" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="W129" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="X129" s="7" t="s">
+        <v>960</v>
+      </c>
+      <c r="Y129" s="7"/>
+      <c r="Z129" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA129" s="7"/>
+      <c r="AB129" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC129" s="9" t="s">
+        <v>961</v>
+      </c>
+      <c r="AD129" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE129" s="7"/>
+      <c r="AF129" s="7"/>
+      <c r="AG129" s="7"/>
+      <c r="AH129" s="7"/>
+      <c r="AI129" s="7"/>
+      <c r="AJ129" s="7"/>
+      <c r="AK129" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="130" spans="1:37">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2026022837</v>
+      </c>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="3"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="3"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="4"/>
+      <c r="Q130" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S130" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T130" s="3">
+        <v>1</v>
+      </c>
+      <c r="U130" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V130" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="W130" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="X130" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="Y130" s="3"/>
+      <c r="Z130" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA130" s="3"/>
+      <c r="AB130" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC130" s="4" t="s">
+        <v>968</v>
+      </c>
+      <c r="AD130" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE130" s="3"/>
+      <c r="AF130" s="3"/>
+      <c r="AG130" s="3"/>
+      <c r="AH130" s="3"/>
+      <c r="AI130" s="3"/>
+      <c r="AJ130" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK130" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02251725
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$130</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$133</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="984">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-25  )</t>
   </si>
@@ -3002,6 +3002,55 @@
   </si>
   <si>
     <t>PMQ1+7210002821</t>
+  </si>
+  <si>
+    <t>1D161115022501</t>
+  </si>
+  <si>
+    <t>2026-02-25 09:12:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/25 09:12 啟動緊急叫修：HUB(DES1210-28)-門市反應全店網路不通，含90、91均不通，請門市重啟數據機+HUB+PEPLINK仍異常，請門市查看設備均有正常過電，HUB 13PORT有插線有亮燈，門市嘗試將數據機的橘色網路線拔除，備援網路也未啟動...須請台芝到店協助確認 PS.2/23中華有到店更換數據機、2/24台芝有到店更換HUB
+</t>
+  </si>
+  <si>
+    <t>2026-02-25 09:17:37</t>
+  </si>
+  <si>
+    <t>2026-02-25 10:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-25 11:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-25 15:17:00</t>
+  </si>
+  <si>
+    <t>1.到場後中華人員表示室內電纜故障，
+中華已排除
+2.PEPLINK 延遲過高，4G容易斷線
+3.已請0800測試PING90、91正常</t>
+  </si>
+  <si>
+    <t>2026-02-25 15:36:27</t>
+  </si>
+  <si>
+    <t>2026-02-25 15:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-25 15:35:00</t>
+  </si>
+  <si>
+    <t>裝潢撤機已完工</t>
+  </si>
+  <si>
+    <t>2026-02-25 15:52:01</t>
+  </si>
+  <si>
+    <t>2026-02-25 15:40:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">裝潢撤機完工 </t>
   </si>
 </sst>
 </file>
@@ -3415,10 +3464,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK130"/>
+  <dimension ref="A1:AK133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC127" sqref="AC127"/>
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14449,7 +14498,7 @@
       <c r="M130" s="4"/>
       <c r="N130" s="3"/>
       <c r="O130" s="4"/>
-      <c r="P130" s="4"/>
+      <c r="P130" s="10"/>
       <c r="Q130" s="3" t="s">
         <v>964</v>
       </c>
@@ -14482,7 +14531,7 @@
       <c r="AB130" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AC130" s="4" t="s">
+      <c r="AC130" s="10" t="s">
         <v>968</v>
       </c>
       <c r="AD130" s="3" t="s">
@@ -14497,6 +14546,257 @@
         <v>61</v>
       </c>
       <c r="AK130" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:37">
+      <c r="A131" s="7">
+        <v>129</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C131" s="7">
+        <v>2026022890</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>969</v>
+      </c>
+      <c r="E131" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>802</v>
+      </c>
+      <c r="G131" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="I131" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="J131" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K131" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L131" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="M131" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N131" s="7">
+        <v>3402</v>
+      </c>
+      <c r="O131" s="8" t="s">
+        <v>805</v>
+      </c>
+      <c r="P131" s="9" t="s">
+        <v>971</v>
+      </c>
+      <c r="Q131" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="R131" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S131" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T131" s="7">
+        <v>1</v>
+      </c>
+      <c r="U131" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V131" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="W131" s="7" t="s">
+        <v>973</v>
+      </c>
+      <c r="X131" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="Y131" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="Z131" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC131" s="9" t="s">
+        <v>976</v>
+      </c>
+      <c r="AD131" s="7"/>
+      <c r="AE131" s="7"/>
+      <c r="AF131" s="7"/>
+      <c r="AG131" s="7"/>
+      <c r="AH131" s="7"/>
+      <c r="AI131" s="7"/>
+      <c r="AJ131" s="7"/>
+      <c r="AK131" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="132" spans="1:37">
+      <c r="A132" s="3">
+        <v>130</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2026022981</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3">
+        <v>2543</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="3"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T132" s="3">
+        <v>1</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="W132" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="X132" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y132" s="3"/>
+      <c r="Z132" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA132" s="3"/>
+      <c r="AB132" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC132" s="10" t="s">
+        <v>980</v>
+      </c>
+      <c r="AD132" s="3"/>
+      <c r="AE132" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF132" s="3"/>
+      <c r="AG132" s="3"/>
+      <c r="AH132" s="3"/>
+      <c r="AI132" s="3"/>
+      <c r="AJ132" s="3"/>
+      <c r="AK132" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="133" spans="1:37">
+      <c r="A133" s="7">
+        <v>131</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C133" s="7">
+        <v>2026023075</v>
+      </c>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7">
+        <v>2543</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="7"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="8"/>
+      <c r="Q133" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="R133" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S133" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T133" s="7">
+        <v>1</v>
+      </c>
+      <c r="U133" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V133" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="W133" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="X133" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA133" s="7"/>
+      <c r="AB133" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC133" s="8" t="s">
+        <v>983</v>
+      </c>
+      <c r="AD133" s="7"/>
+      <c r="AE133" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF133" s="7"/>
+      <c r="AG133" s="7"/>
+      <c r="AH133" s="7"/>
+      <c r="AI133" s="7"/>
+      <c r="AJ133" s="7"/>
+      <c r="AK133" s="7" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit - 02261724
</commit_message>
<xml_diff>
--- a/IM/202602_HL_Maintain_Report.xlsx
+++ b/IM/202602_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$133</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$156</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="984">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-25  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1113">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202602   (  製表日期:2026-02-26  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -3004,6 +3004,30 @@
     <t>PMQ1+7210002821</t>
   </si>
   <si>
+    <t>12570115022401</t>
+  </si>
+  <si>
+    <t>2026-02-24 18:57:53</t>
+  </si>
+  <si>
+    <t>門市反應LIFE ET印票機(L90)亮紅燈、無法刷讀小白單，確認卷紙充足，長按電源鍵無反應、現場線路繁亂無法重新插拔電源線...需請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2026-02-24 19:00:32</t>
+  </si>
+  <si>
+    <t>2026-02-25 16:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-25 17:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-25 23:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">重新插拔網路變壓器插座    </t>
+  </si>
+  <si>
     <t>1D161115022501</t>
   </si>
   <si>
@@ -3032,6 +3056,69 @@
 3.已請0800測試PING90、91正常</t>
   </si>
   <si>
+    <t>12315115022501</t>
+  </si>
+  <si>
+    <t>蘆竹坑口店</t>
+  </si>
+  <si>
+    <t>2026-02-25 10:04:46</t>
+  </si>
+  <si>
+    <t>開機異常、反覆重開機</t>
+  </si>
+  <si>
+    <t>門市反應mmk4代機昨天停電復電後無法開機，按電源鍵無反應ping60不通，門市不願意協助排除....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02315</t>
+  </si>
+  <si>
+    <t>2026-02-25 10:06:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:30:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 12:27:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 14:06:00</t>
+  </si>
+  <si>
+    <t>需強制關機後重新啟動，目前測試皆為正常</t>
+  </si>
+  <si>
+    <t>15384115022501</t>
+  </si>
+  <si>
+    <t>板橋民生站</t>
+  </si>
+  <si>
+    <t>2026-02-25 14:45:22</t>
+  </si>
+  <si>
+    <t>門市反應TM2(TCX800)觸控延遲，與門市確認TM無張貼文宣及透明塑膠墊，已嘗試執行觸控校正仍無改善..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05384</t>
+  </si>
+  <si>
+    <t>2026-02-25 14:47:28</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:45:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 18:47:00</t>
+  </si>
+  <si>
+    <t>線路重新插拔，軟體校正後測試正常</t>
+  </si>
+  <si>
     <t>2026-02-25 15:36:27</t>
   </si>
   <si>
@@ -3051,6 +3138,306 @@
   </si>
   <si>
     <t xml:space="preserve">裝潢撤機完工 </t>
+  </si>
+  <si>
+    <t>2026-02-25 17:38:31</t>
+  </si>
+  <si>
+    <t>2026-02-25 17:30:00</t>
+  </si>
+  <si>
+    <t>三重仁旺店</t>
+  </si>
+  <si>
+    <t>THILF04397</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:53:25</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:27:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:48:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002803</t>
+  </si>
+  <si>
+    <t>新莊小胖店</t>
+  </si>
+  <si>
+    <t>THILF04856</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:53:38</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:00:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003068+L90</t>
+  </si>
+  <si>
+    <t>新莊祐信店</t>
+  </si>
+  <si>
+    <t>THILF04025</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:05:42</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:40:00</t>
+  </si>
+  <si>
+    <t>三重義天店</t>
+  </si>
+  <si>
+    <t>THILF02222</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:20:35</t>
+  </si>
+  <si>
+    <t>2026-02-26 09:56:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:16:00</t>
+  </si>
+  <si>
+    <t>新莊中港店</t>
+  </si>
+  <si>
+    <t>THILF05057</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:20:43</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003069+L90</t>
+  </si>
+  <si>
+    <t>新莊莊民店</t>
+  </si>
+  <si>
+    <t>THILF03652</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:30:19</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003055</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:48:50</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:28:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:43:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002863</t>
+  </si>
+  <si>
+    <t>D195</t>
+  </si>
+  <si>
+    <t>三重車路頭</t>
+  </si>
+  <si>
+    <t>THILF0D195</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:54:03</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:25:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002822</t>
+  </si>
+  <si>
+    <t>新莊化成店</t>
+  </si>
+  <si>
+    <t>THILF02362</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:58:47</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:40:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003050</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:09:23</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:00:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003060+L90</t>
+  </si>
+  <si>
+    <t>新莊鼎苑店</t>
+  </si>
+  <si>
+    <t>THILF04194</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:35:12</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:20:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210003062</t>
+  </si>
+  <si>
+    <t>三重薔薇店</t>
+  </si>
+  <si>
+    <t>THILF04388</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:36:52</t>
+  </si>
+  <si>
+    <t>2026-02-26 10:57:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:18:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002802</t>
+  </si>
+  <si>
+    <t>三重重新橋</t>
+  </si>
+  <si>
+    <t>THILF03627</t>
+  </si>
+  <si>
+    <t>2026-02-26 12:33:12</t>
+  </si>
+  <si>
+    <t>2026-02-26 11:50:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 12:10:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 12:33:16</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002776</t>
+  </si>
+  <si>
+    <t>三重商工店</t>
+  </si>
+  <si>
+    <t>THILF04652</t>
+  </si>
+  <si>
+    <t>2026-02-26 14:34:03</t>
+  </si>
+  <si>
+    <t>2026-02-26 13:42:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 14:03:00</t>
+  </si>
+  <si>
+    <t>三重太璞宮</t>
+  </si>
+  <si>
+    <t>THILF04968</t>
+  </si>
+  <si>
+    <t>2026-02-26 14:56:55</t>
+  </si>
+  <si>
+    <t>2026-02-26 14:15:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 14:37:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002808</t>
+  </si>
+  <si>
+    <t>D390</t>
+  </si>
+  <si>
+    <t>三重大有店</t>
+  </si>
+  <si>
+    <t>THILF0D390</t>
+  </si>
+  <si>
+    <t>2026-02-26 15:25:59</t>
+  </si>
+  <si>
+    <t>2026-02-26 14:48:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 15:10:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002824</t>
+  </si>
+  <si>
+    <t>D024</t>
+  </si>
+  <si>
+    <t>三重三民店</t>
+  </si>
+  <si>
+    <t>THILF0D024</t>
+  </si>
+  <si>
+    <t>2026-02-26 15:59:15</t>
+  </si>
+  <si>
+    <t>2026-02-26 15:25:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 15:47:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002814</t>
+  </si>
+  <si>
+    <t>三重星光店</t>
+  </si>
+  <si>
+    <t>THILF03983</t>
+  </si>
+  <si>
+    <t>2026-02-26 16:58:04</t>
+  </si>
+  <si>
+    <t>2026-02-26 16:41:00</t>
+  </si>
+  <si>
+    <t>2026-02-26 16:56:00</t>
+  </si>
+  <si>
+    <t>PMQ1+7210002784</t>
   </si>
 </sst>
 </file>
@@ -3464,10 +3851,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK133"/>
+  <dimension ref="A1:AK156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A133" sqref="A133"/>
+      <selection activeCell="AC153" sqref="AC153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14557,55 +14944,55 @@
         <v>38</v>
       </c>
       <c r="C131" s="7">
-        <v>2026022890</v>
+        <v>2026022874</v>
       </c>
       <c r="D131" s="7" t="s">
         <v>969</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>470</v>
-      </c>
-      <c r="F131" s="7" t="s">
-        <v>802</v>
+        <v>40</v>
+      </c>
+      <c r="F131" s="7">
+        <v>2570</v>
       </c>
       <c r="G131" s="7" t="s">
-        <v>803</v>
+        <v>305</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>244</v>
+        <v>65</v>
       </c>
       <c r="I131" s="7" t="s">
         <v>970</v>
       </c>
       <c r="J131" s="7" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="K131" s="7" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="L131" s="7" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="M131" s="8" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="N131" s="7">
-        <v>3402</v>
+        <v>6003</v>
       </c>
       <c r="O131" s="8" t="s">
-        <v>805</v>
+        <v>505</v>
       </c>
       <c r="P131" s="9" t="s">
         <v>971</v>
       </c>
       <c r="Q131" s="7" t="s">
-        <v>807</v>
+        <v>306</v>
       </c>
       <c r="R131" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S131" s="7" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="T131" s="7">
         <v>1</v>
@@ -14626,7 +15013,7 @@
         <v>975</v>
       </c>
       <c r="Z131" s="7">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="AA131" s="7"/>
       <c r="AB131" s="7" t="s">
@@ -14651,38 +15038,58 @@
         <v>130</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C132" s="3">
-        <v>2026022981</v>
-      </c>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
-      <c r="F132" s="3">
-        <v>2543</v>
+        <v>2026022890</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>802</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>329</v>
+        <v>803</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I132" s="3"/>
-      <c r="J132" s="3"/>
-      <c r="K132" s="3"/>
-      <c r="L132" s="3"/>
-      <c r="M132" s="4"/>
-      <c r="N132" s="3"/>
-      <c r="O132" s="4"/>
-      <c r="P132" s="10"/>
+        <v>244</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K132" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L132" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M132" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="N132" s="3">
+        <v>3402</v>
+      </c>
+      <c r="O132" s="4" t="s">
+        <v>805</v>
+      </c>
+      <c r="P132" s="10" t="s">
+        <v>979</v>
+      </c>
       <c r="Q132" s="3" t="s">
-        <v>330</v>
+        <v>807</v>
       </c>
       <c r="R132" s="3" t="s">
         <v>52</v>
       </c>
       <c r="S132" s="3" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="T132" s="3">
         <v>1</v>
@@ -14691,29 +15098,29 @@
         <v>54</v>
       </c>
       <c r="V132" s="3" t="s">
-        <v>977</v>
+        <v>980</v>
       </c>
       <c r="W132" s="3" t="s">
-        <v>978</v>
+        <v>981</v>
       </c>
       <c r="X132" s="3" t="s">
-        <v>979</v>
-      </c>
-      <c r="Y132" s="3"/>
+        <v>982</v>
+      </c>
+      <c r="Y132" s="3" t="s">
+        <v>983</v>
+      </c>
       <c r="Z132" s="3">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="AA132" s="3"/>
       <c r="AB132" s="3" t="s">
         <v>59</v>
       </c>
       <c r="AC132" s="10" t="s">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="AD132" s="3"/>
-      <c r="AE132" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="AE132" s="3"/>
       <c r="AF132" s="3"/>
       <c r="AG132" s="3"/>
       <c r="AH132" s="3"/>
@@ -14728,38 +15135,58 @@
         <v>131</v>
       </c>
       <c r="B133" s="7" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C133" s="7">
-        <v>2026023075</v>
-      </c>
-      <c r="D133" s="7"/>
-      <c r="E133" s="7"/>
+        <v>2026022919</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>985</v>
+      </c>
+      <c r="E133" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F133" s="7">
-        <v>2543</v>
+        <v>2315</v>
       </c>
       <c r="G133" s="7" t="s">
-        <v>329</v>
+        <v>986</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I133" s="7"/>
-      <c r="J133" s="7"/>
-      <c r="K133" s="7"/>
-      <c r="L133" s="7"/>
-      <c r="M133" s="8"/>
-      <c r="N133" s="7"/>
-      <c r="O133" s="8"/>
-      <c r="P133" s="8"/>
+        <v>172</v>
+      </c>
+      <c r="I133" s="7" t="s">
+        <v>987</v>
+      </c>
+      <c r="J133" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="K133" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L133" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M133" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="N133" s="7">
+        <v>5805</v>
+      </c>
+      <c r="O133" s="8" t="s">
+        <v>988</v>
+      </c>
+      <c r="P133" s="9" t="s">
+        <v>989</v>
+      </c>
       <c r="Q133" s="7" t="s">
-        <v>330</v>
+        <v>990</v>
       </c>
       <c r="R133" s="7" t="s">
         <v>52</v>
       </c>
       <c r="S133" s="7" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="T133" s="7">
         <v>1</v>
@@ -14768,35 +15195,1852 @@
         <v>54</v>
       </c>
       <c r="V133" s="7" t="s">
-        <v>981</v>
+        <v>991</v>
       </c>
       <c r="W133" s="7" t="s">
-        <v>978</v>
+        <v>992</v>
       </c>
       <c r="X133" s="7" t="s">
-        <v>982</v>
-      </c>
-      <c r="Y133" s="7"/>
+        <v>993</v>
+      </c>
+      <c r="Y133" s="7" t="s">
+        <v>994</v>
+      </c>
       <c r="Z133" s="7">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="AA133" s="7"/>
       <c r="AB133" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC133" s="8" t="s">
-        <v>983</v>
+      <c r="AC133" s="9" t="s">
+        <v>995</v>
       </c>
       <c r="AD133" s="7"/>
-      <c r="AE133" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="AE133" s="7"/>
       <c r="AF133" s="7"/>
       <c r="AG133" s="7"/>
       <c r="AH133" s="7"/>
       <c r="AI133" s="7"/>
       <c r="AJ133" s="7"/>
       <c r="AK133" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="134" spans="1:37">
+      <c r="A134" s="3">
+        <v>132</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2026022967</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" s="3">
+        <v>5384</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M134" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N134" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O134" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="P134" s="10" t="s">
+        <v>999</v>
+      </c>
+      <c r="Q134" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R134" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S134" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T134" s="3">
+        <v>1</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V134" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="W134" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="X134" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="Y134" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="Z134" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA134" s="3"/>
+      <c r="AB134" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC134" s="10" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AD134" s="3"/>
+      <c r="AE134" s="3"/>
+      <c r="AF134" s="3"/>
+      <c r="AG134" s="3"/>
+      <c r="AH134" s="3"/>
+      <c r="AI134" s="3"/>
+      <c r="AJ134" s="3"/>
+      <c r="AK134" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="135" spans="1:37">
+      <c r="A135" s="7">
+        <v>133</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C135" s="7">
+        <v>2026022981</v>
+      </c>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="7">
+        <v>2543</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I135" s="7"/>
+      <c r="J135" s="7"/>
+      <c r="K135" s="7"/>
+      <c r="L135" s="7"/>
+      <c r="M135" s="8"/>
+      <c r="N135" s="7"/>
+      <c r="O135" s="8"/>
+      <c r="P135" s="9"/>
+      <c r="Q135" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="R135" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S135" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T135" s="7">
+        <v>1</v>
+      </c>
+      <c r="U135" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V135" s="7" t="s">
+        <v>1006</v>
+      </c>
+      <c r="W135" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="X135" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Y135" s="7"/>
+      <c r="Z135" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA135" s="7"/>
+      <c r="AB135" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC135" s="9" t="s">
+        <v>1009</v>
+      </c>
+      <c r="AD135" s="7"/>
+      <c r="AE135" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF135" s="7"/>
+      <c r="AG135" s="7"/>
+      <c r="AH135" s="7"/>
+      <c r="AI135" s="7"/>
+      <c r="AJ135" s="7"/>
+      <c r="AK135" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="136" spans="1:37">
+      <c r="A136" s="3">
+        <v>134</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C136" s="3">
+        <v>2026023075</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3">
+        <v>2543</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I136" s="3"/>
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="3"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="3"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="10"/>
+      <c r="Q136" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="R136" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S136" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T136" s="3">
+        <v>1</v>
+      </c>
+      <c r="U136" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V136" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="W136" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="X136" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Y136" s="3"/>
+      <c r="Z136" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA136" s="3"/>
+      <c r="AB136" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC136" s="10" t="s">
+        <v>1012</v>
+      </c>
+      <c r="AD136" s="3"/>
+      <c r="AE136" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF136" s="3"/>
+      <c r="AG136" s="3"/>
+      <c r="AH136" s="3"/>
+      <c r="AI136" s="3"/>
+      <c r="AJ136" s="3"/>
+      <c r="AK136" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="137" spans="1:37">
+      <c r="A137" s="7">
+        <v>135</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C137" s="7">
+        <v>2026023113</v>
+      </c>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7">
+        <v>2570</v>
+      </c>
+      <c r="G137" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I137" s="7"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
+      <c r="L137" s="7"/>
+      <c r="M137" s="8"/>
+      <c r="N137" s="7"/>
+      <c r="O137" s="8"/>
+      <c r="P137" s="9"/>
+      <c r="Q137" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="R137" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S137" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T137" s="7">
+        <v>1</v>
+      </c>
+      <c r="U137" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V137" s="7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="W137" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="X137" s="7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="Y137" s="7"/>
+      <c r="Z137" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA137" s="7"/>
+      <c r="AB137" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC137" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="AD137" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE137" s="7"/>
+      <c r="AF137" s="7"/>
+      <c r="AG137" s="7"/>
+      <c r="AH137" s="7"/>
+      <c r="AI137" s="7"/>
+      <c r="AJ137" s="7"/>
+      <c r="AK137" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="138" spans="1:37">
+      <c r="A138" s="3">
+        <v>136</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C138" s="3">
+        <v>2026023127</v>
+      </c>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3">
+        <v>4397</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
+      <c r="M138" s="4"/>
+      <c r="N138" s="3"/>
+      <c r="O138" s="4"/>
+      <c r="P138" s="10"/>
+      <c r="Q138" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="R138" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S138" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T138" s="3">
+        <v>1</v>
+      </c>
+      <c r="U138" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V138" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="W138" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="X138" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="Y138" s="3"/>
+      <c r="Z138" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA138" s="3"/>
+      <c r="AB138" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC138" s="10" t="s">
+        <v>1020</v>
+      </c>
+      <c r="AD138" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE138" s="3"/>
+      <c r="AF138" s="3"/>
+      <c r="AG138" s="3"/>
+      <c r="AH138" s="3"/>
+      <c r="AI138" s="3"/>
+      <c r="AJ138" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK138" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="139" spans="1:37">
+      <c r="A139" s="7">
+        <v>137</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C139" s="7">
+        <v>2026023128</v>
+      </c>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
+      <c r="F139" s="7">
+        <v>4856</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>1021</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I139" s="7"/>
+      <c r="J139" s="7"/>
+      <c r="K139" s="7"/>
+      <c r="L139" s="7"/>
+      <c r="M139" s="8"/>
+      <c r="N139" s="7"/>
+      <c r="O139" s="8"/>
+      <c r="P139" s="9"/>
+      <c r="Q139" s="7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="R139" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S139" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T139" s="7">
+        <v>1</v>
+      </c>
+      <c r="U139" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V139" s="7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="W139" s="7" t="s">
+        <v>1024</v>
+      </c>
+      <c r="X139" s="7" t="s">
+        <v>1025</v>
+      </c>
+      <c r="Y139" s="7"/>
+      <c r="Z139" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA139" s="7"/>
+      <c r="AB139" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC139" s="9" t="s">
+        <v>1026</v>
+      </c>
+      <c r="AD139" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE139" s="7"/>
+      <c r="AF139" s="7"/>
+      <c r="AG139" s="7"/>
+      <c r="AH139" s="7"/>
+      <c r="AI139" s="7"/>
+      <c r="AJ139" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK139" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="140" spans="1:37">
+      <c r="A140" s="3">
+        <v>138</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C140" s="3">
+        <v>2026023132</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3">
+        <v>4025</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="R140" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S140" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T140" s="3">
+        <v>1</v>
+      </c>
+      <c r="U140" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V140" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="W140" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="X140" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="Y140" s="3"/>
+      <c r="Z140" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA140" s="3"/>
+      <c r="AB140" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC140" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD140" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE140" s="3"/>
+      <c r="AF140" s="3"/>
+      <c r="AG140" s="3"/>
+      <c r="AH140" s="3"/>
+      <c r="AI140" s="3"/>
+      <c r="AJ140" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK140" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="141" spans="1:37">
+      <c r="A141" s="7">
+        <v>139</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C141" s="7">
+        <v>2026023135</v>
+      </c>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7">
+        <v>2222</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I141" s="7"/>
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
+      <c r="L141" s="7"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="7"/>
+      <c r="O141" s="8"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="7" t="s">
+        <v>1032</v>
+      </c>
+      <c r="R141" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S141" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T141" s="7">
+        <v>1</v>
+      </c>
+      <c r="U141" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V141" s="7" t="s">
+        <v>1033</v>
+      </c>
+      <c r="W141" s="7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="X141" s="7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="Y141" s="7"/>
+      <c r="Z141" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA141" s="7"/>
+      <c r="AB141" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC141" s="9" t="s">
+        <v>876</v>
+      </c>
+      <c r="AD141" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE141" s="7"/>
+      <c r="AF141" s="7"/>
+      <c r="AG141" s="7"/>
+      <c r="AH141" s="7"/>
+      <c r="AI141" s="7"/>
+      <c r="AJ141" s="7"/>
+      <c r="AK141" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="142" spans="1:37">
+      <c r="A142" s="3">
+        <v>140</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2026023136</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3">
+        <v>5057</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="10"/>
+      <c r="Q142" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="R142" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S142" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T142" s="3">
+        <v>1</v>
+      </c>
+      <c r="U142" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V142" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="W142" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="X142" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="Y142" s="3"/>
+      <c r="Z142" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA142" s="3"/>
+      <c r="AB142" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC142" s="10" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AD142" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE142" s="3"/>
+      <c r="AF142" s="3"/>
+      <c r="AG142" s="3"/>
+      <c r="AH142" s="3"/>
+      <c r="AI142" s="3"/>
+      <c r="AJ142" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK142" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="143" spans="1:37">
+      <c r="A143" s="7">
+        <v>141</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C143" s="7">
+        <v>2026023157</v>
+      </c>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7">
+        <v>3652</v>
+      </c>
+      <c r="G143" s="7" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H143" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I143" s="7"/>
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="8"/>
+      <c r="N143" s="7"/>
+      <c r="O143" s="8"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="7" t="s">
+        <v>1042</v>
+      </c>
+      <c r="R143" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S143" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T143" s="7">
+        <v>1</v>
+      </c>
+      <c r="U143" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V143" s="7" t="s">
+        <v>1043</v>
+      </c>
+      <c r="W143" s="7" t="s">
+        <v>1039</v>
+      </c>
+      <c r="X143" s="7" t="s">
+        <v>1044</v>
+      </c>
+      <c r="Y143" s="7"/>
+      <c r="Z143" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA143" s="7"/>
+      <c r="AB143" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC143" s="9" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AD143" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE143" s="7"/>
+      <c r="AF143" s="7"/>
+      <c r="AG143" s="7"/>
+      <c r="AH143" s="7"/>
+      <c r="AI143" s="7"/>
+      <c r="AJ143" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK143" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:37">
+      <c r="A144" s="3">
+        <v>142</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C144" s="3">
+        <v>2026023169</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3">
+        <v>5384</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="10"/>
+      <c r="Q144" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R144" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S144" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="T144" s="3">
+        <v>1</v>
+      </c>
+      <c r="U144" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V144" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="W144" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="X144" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="Y144" s="3"/>
+      <c r="Z144" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA144" s="3"/>
+      <c r="AB144" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC144" s="10" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AD144" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE144" s="3"/>
+      <c r="AF144" s="3"/>
+      <c r="AG144" s="3"/>
+      <c r="AH144" s="3"/>
+      <c r="AI144" s="3"/>
+      <c r="AJ144" s="3"/>
+      <c r="AK144" s="3"/>
+    </row>
+    <row r="145" spans="1:37">
+      <c r="A145" s="7">
+        <v>143</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C145" s="7">
+        <v>2026023171</v>
+      </c>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7" t="s">
+        <v>1050</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I145" s="7"/>
+      <c r="J145" s="7"/>
+      <c r="K145" s="7"/>
+      <c r="L145" s="7"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="7"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="9"/>
+      <c r="Q145" s="7" t="s">
+        <v>1052</v>
+      </c>
+      <c r="R145" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S145" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T145" s="7">
+        <v>1</v>
+      </c>
+      <c r="U145" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V145" s="7" t="s">
+        <v>1053</v>
+      </c>
+      <c r="W145" s="7" t="s">
+        <v>1054</v>
+      </c>
+      <c r="X145" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="Y145" s="7"/>
+      <c r="Z145" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA145" s="7"/>
+      <c r="AB145" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC145" s="9" t="s">
+        <v>1055</v>
+      </c>
+      <c r="AD145" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE145" s="7"/>
+      <c r="AF145" s="7"/>
+      <c r="AG145" s="7"/>
+      <c r="AH145" s="7"/>
+      <c r="AI145" s="7"/>
+      <c r="AJ145" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK145" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="146" spans="1:37">
+      <c r="A146" s="3">
+        <v>144</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2026023172</v>
+      </c>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3">
+        <v>2362</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="4"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="4"/>
+      <c r="P146" s="10"/>
+      <c r="Q146" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="R146" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S146" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T146" s="3">
+        <v>1</v>
+      </c>
+      <c r="U146" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V146" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="W146" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="X146" s="3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Y146" s="3"/>
+      <c r="Z146" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA146" s="3"/>
+      <c r="AB146" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC146" s="10" t="s">
+        <v>1060</v>
+      </c>
+      <c r="AD146" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE146" s="3"/>
+      <c r="AF146" s="3"/>
+      <c r="AG146" s="3"/>
+      <c r="AH146" s="3"/>
+      <c r="AI146" s="3"/>
+      <c r="AJ146" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK146" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="147" spans="1:37">
+      <c r="A147" s="7">
+        <v>145</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C147" s="7">
+        <v>2026023174</v>
+      </c>
+      <c r="D147" s="7"/>
+      <c r="E147" s="7"/>
+      <c r="F147" s="7">
+        <v>4144</v>
+      </c>
+      <c r="G147" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I147" s="7"/>
+      <c r="J147" s="7"/>
+      <c r="K147" s="7"/>
+      <c r="L147" s="7"/>
+      <c r="M147" s="8"/>
+      <c r="N147" s="7"/>
+      <c r="O147" s="8"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="R147" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S147" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="T147" s="7">
+        <v>1</v>
+      </c>
+      <c r="U147" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V147" s="7" t="s">
+        <v>1061</v>
+      </c>
+      <c r="W147" s="7" t="s">
+        <v>1059</v>
+      </c>
+      <c r="X147" s="7" t="s">
+        <v>1062</v>
+      </c>
+      <c r="Y147" s="7"/>
+      <c r="Z147" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA147" s="7"/>
+      <c r="AB147" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC147" s="9" t="s">
+        <v>1063</v>
+      </c>
+      <c r="AD147" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE147" s="7"/>
+      <c r="AF147" s="7"/>
+      <c r="AG147" s="7"/>
+      <c r="AH147" s="7"/>
+      <c r="AI147" s="7"/>
+      <c r="AJ147" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK147" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="148" spans="1:37">
+      <c r="A148" s="3">
+        <v>146</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C148" s="3">
+        <v>2026023177</v>
+      </c>
+      <c r="D148" s="3"/>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3">
+        <v>4194</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I148" s="3"/>
+      <c r="J148" s="3"/>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="4"/>
+      <c r="N148" s="3"/>
+      <c r="O148" s="4"/>
+      <c r="P148" s="10"/>
+      <c r="Q148" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="R148" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S148" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="T148" s="3">
+        <v>1</v>
+      </c>
+      <c r="U148" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V148" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="W148" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="X148" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="Y148" s="3"/>
+      <c r="Z148" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA148" s="3"/>
+      <c r="AB148" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC148" s="10" t="s">
+        <v>1068</v>
+      </c>
+      <c r="AD148" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE148" s="3"/>
+      <c r="AF148" s="3"/>
+      <c r="AG148" s="3"/>
+      <c r="AH148" s="3"/>
+      <c r="AI148" s="3"/>
+      <c r="AJ148" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK148" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="149" spans="1:37">
+      <c r="A149" s="7">
+        <v>147</v>
+      </c>
+      <c r="B149" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C149" s="7">
+        <v>2026023178</v>
+      </c>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="7">
+        <v>4388</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H149" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I149" s="7"/>
+      <c r="J149" s="7"/>
+      <c r="K149" s="7"/>
+      <c r="L149" s="7"/>
+      <c r="M149" s="8"/>
+      <c r="N149" s="7"/>
+      <c r="O149" s="8"/>
+      <c r="P149" s="9"/>
+      <c r="Q149" s="7" t="s">
+        <v>1070</v>
+      </c>
+      <c r="R149" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S149" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T149" s="7">
+        <v>1</v>
+      </c>
+      <c r="U149" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V149" s="7" t="s">
+        <v>1071</v>
+      </c>
+      <c r="W149" s="7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="X149" s="7" t="s">
+        <v>1073</v>
+      </c>
+      <c r="Y149" s="7"/>
+      <c r="Z149" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA149" s="7"/>
+      <c r="AB149" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC149" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="AD149" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE149" s="7"/>
+      <c r="AF149" s="7"/>
+      <c r="AG149" s="7"/>
+      <c r="AH149" s="7"/>
+      <c r="AI149" s="7"/>
+      <c r="AJ149" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK149" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="150" spans="1:37">
+      <c r="A150" s="3">
+        <v>148</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C150" s="3">
+        <v>2026023192</v>
+      </c>
+      <c r="D150" s="3"/>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3">
+        <v>3627</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I150" s="3"/>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="4"/>
+      <c r="N150" s="3"/>
+      <c r="O150" s="4"/>
+      <c r="P150" s="10"/>
+      <c r="Q150" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="R150" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S150" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T150" s="3">
+        <v>1</v>
+      </c>
+      <c r="U150" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V150" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="W150" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="X150" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="Y150" s="3"/>
+      <c r="Z150" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA150" s="3"/>
+      <c r="AB150" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC150" s="10" t="s">
+        <v>876</v>
+      </c>
+      <c r="AD150" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE150" s="3"/>
+      <c r="AF150" s="3"/>
+      <c r="AG150" s="3"/>
+      <c r="AH150" s="3"/>
+      <c r="AI150" s="3"/>
+      <c r="AJ150" s="3"/>
+      <c r="AK150" s="3"/>
+    </row>
+    <row r="151" spans="1:37">
+      <c r="A151" s="7">
+        <v>149</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C151" s="7">
+        <v>2026023193</v>
+      </c>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
+      <c r="F151" s="7">
+        <v>3627</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="H151" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I151" s="7"/>
+      <c r="J151" s="7"/>
+      <c r="K151" s="7"/>
+      <c r="L151" s="7"/>
+      <c r="M151" s="8"/>
+      <c r="N151" s="7"/>
+      <c r="O151" s="8"/>
+      <c r="P151" s="9"/>
+      <c r="Q151" s="7" t="s">
+        <v>1076</v>
+      </c>
+      <c r="R151" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S151" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T151" s="7">
+        <v>1</v>
+      </c>
+      <c r="U151" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V151" s="7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="W151" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="X151" s="7" t="s">
+        <v>1078</v>
+      </c>
+      <c r="Y151" s="7"/>
+      <c r="Z151" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA151" s="7"/>
+      <c r="AB151" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC151" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="AD151" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE151" s="7"/>
+      <c r="AF151" s="7"/>
+      <c r="AG151" s="7"/>
+      <c r="AH151" s="7"/>
+      <c r="AI151" s="7"/>
+      <c r="AJ151" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK151" s="7"/>
+    </row>
+    <row r="152" spans="1:37">
+      <c r="A152" s="3">
+        <v>150</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C152" s="3">
+        <v>2026023209</v>
+      </c>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3">
+        <v>4652</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I152" s="3"/>
+      <c r="J152" s="3"/>
+      <c r="K152" s="3"/>
+      <c r="L152" s="3"/>
+      <c r="M152" s="4"/>
+      <c r="N152" s="3"/>
+      <c r="O152" s="4"/>
+      <c r="P152" s="10"/>
+      <c r="Q152" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="R152" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S152" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T152" s="3">
+        <v>1</v>
+      </c>
+      <c r="U152" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V152" s="3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="W152" s="3" t="s">
+        <v>1085</v>
+      </c>
+      <c r="X152" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="Y152" s="3"/>
+      <c r="Z152" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA152" s="3"/>
+      <c r="AB152" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC152" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD152" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE152" s="3"/>
+      <c r="AF152" s="3"/>
+      <c r="AG152" s="3"/>
+      <c r="AH152" s="3"/>
+      <c r="AI152" s="3"/>
+      <c r="AJ152" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK152" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:37">
+      <c r="A153" s="7">
+        <v>151</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C153" s="7">
+        <v>2026023216</v>
+      </c>
+      <c r="D153" s="7"/>
+      <c r="E153" s="7"/>
+      <c r="F153" s="7">
+        <v>4968</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>1087</v>
+      </c>
+      <c r="H153" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I153" s="7"/>
+      <c r="J153" s="7"/>
+      <c r="K153" s="7"/>
+      <c r="L153" s="7"/>
+      <c r="M153" s="8"/>
+      <c r="N153" s="7"/>
+      <c r="O153" s="8"/>
+      <c r="P153" s="9"/>
+      <c r="Q153" s="7" t="s">
+        <v>1088</v>
+      </c>
+      <c r="R153" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S153" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T153" s="7">
+        <v>1</v>
+      </c>
+      <c r="U153" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V153" s="7" t="s">
+        <v>1089</v>
+      </c>
+      <c r="W153" s="7" t="s">
+        <v>1090</v>
+      </c>
+      <c r="X153" s="7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="Y153" s="7"/>
+      <c r="Z153" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA153" s="7"/>
+      <c r="AB153" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC153" s="9" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AD153" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE153" s="7"/>
+      <c r="AF153" s="7"/>
+      <c r="AG153" s="7"/>
+      <c r="AH153" s="7"/>
+      <c r="AI153" s="7"/>
+      <c r="AJ153" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK153" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="154" spans="1:37">
+      <c r="A154" s="3">
+        <v>152</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C154" s="3">
+        <v>2026023223</v>
+      </c>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I154" s="3"/>
+      <c r="J154" s="3"/>
+      <c r="K154" s="3"/>
+      <c r="L154" s="3"/>
+      <c r="M154" s="4"/>
+      <c r="N154" s="3"/>
+      <c r="O154" s="4"/>
+      <c r="P154" s="10"/>
+      <c r="Q154" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="R154" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S154" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T154" s="3">
+        <v>1</v>
+      </c>
+      <c r="U154" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V154" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="W154" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="X154" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="Y154" s="3"/>
+      <c r="Z154" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA154" s="3"/>
+      <c r="AB154" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC154" s="10" t="s">
+        <v>1099</v>
+      </c>
+      <c r="AD154" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE154" s="3"/>
+      <c r="AF154" s="3"/>
+      <c r="AG154" s="3"/>
+      <c r="AH154" s="3"/>
+      <c r="AI154" s="3"/>
+      <c r="AJ154" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK154" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="155" spans="1:37">
+      <c r="A155" s="7">
+        <v>153</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C155" s="7">
+        <v>2026023227</v>
+      </c>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7" t="s">
+        <v>1100</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>1101</v>
+      </c>
+      <c r="H155" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I155" s="7"/>
+      <c r="J155" s="7"/>
+      <c r="K155" s="7"/>
+      <c r="L155" s="7"/>
+      <c r="M155" s="8"/>
+      <c r="N155" s="7"/>
+      <c r="O155" s="8"/>
+      <c r="P155" s="9"/>
+      <c r="Q155" s="7" t="s">
+        <v>1102</v>
+      </c>
+      <c r="R155" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S155" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T155" s="7">
+        <v>1</v>
+      </c>
+      <c r="U155" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="V155" s="7" t="s">
+        <v>1103</v>
+      </c>
+      <c r="W155" s="7" t="s">
+        <v>1104</v>
+      </c>
+      <c r="X155" s="7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="Y155" s="7"/>
+      <c r="Z155" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA155" s="7"/>
+      <c r="AB155" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC155" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="AD155" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE155" s="7"/>
+      <c r="AF155" s="7"/>
+      <c r="AG155" s="7"/>
+      <c r="AH155" s="7"/>
+      <c r="AI155" s="7"/>
+      <c r="AJ155" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK155" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="156" spans="1:37">
+      <c r="A156" s="3">
+        <v>154</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C156" s="3">
+        <v>2026023293</v>
+      </c>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
+      <c r="F156" s="3">
+        <v>3983</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I156" s="3"/>
+      <c r="J156" s="3"/>
+      <c r="K156" s="3"/>
+      <c r="L156" s="3"/>
+      <c r="M156" s="4"/>
+      <c r="N156" s="3"/>
+      <c r="O156" s="4"/>
+      <c r="P156" s="4"/>
+      <c r="Q156" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="R156" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S156" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T156" s="3">
+        <v>1</v>
+      </c>
+      <c r="U156" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="V156" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="W156" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="X156" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="Y156" s="3"/>
+      <c r="Z156" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA156" s="3"/>
+      <c r="AB156" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC156" s="4" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AD156" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE156" s="3"/>
+      <c r="AF156" s="3"/>
+      <c r="AG156" s="3"/>
+      <c r="AH156" s="3"/>
+      <c r="AI156" s="3"/>
+      <c r="AJ156" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK156" s="3" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>